<commit_message>
Added test results for iOS Safari
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC760D1-A26C-7141-BAEF-1C77718C38D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947A2AE-6961-744C-98FA-1A87C48AAADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="28200" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="96">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -285,13 +285,34 @@
   </si>
   <si>
     <t>spoken by VoiceOver</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>region, landmark</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>navigation, landmark</t>
+  </si>
+  <si>
+    <t>note, landmark</t>
+  </si>
+  <si>
+    <t>cannot focus on it</t>
+  </si>
+  <si>
+    <t>heading level 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +322,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -364,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -373,16 +409,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -729,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,65 +801,72 @@
     <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="4" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q2" s="13"/>
+      <c r="R2" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -867,8 +918,11 @@
       <c r="Q3" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -920,8 +974,11 @@
       <c r="Q4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -973,8 +1030,11 @@
       <c r="Q5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1026,8 +1086,11 @@
       <c r="Q6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1079,8 +1142,11 @@
       <c r="Q7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1132,8 +1198,11 @@
       <c r="Q8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1185,8 +1254,11 @@
       <c r="Q9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1238,8 +1310,11 @@
       <c r="Q10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1291,8 +1366,11 @@
       <c r="Q11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R11" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1344,8 +1422,11 @@
       <c r="Q12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1397,8 +1478,11 @@
       <c r="Q13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1450,8 +1534,11 @@
       <c r="Q14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1503,8 +1590,11 @@
       <c r="Q15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1556,8 +1646,11 @@
       <c r="Q16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1609,8 +1702,11 @@
       <c r="Q17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1662,8 +1758,11 @@
       <c r="Q18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1715,8 +1814,11 @@
       <c r="Q19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1768,8 +1870,11 @@
       <c r="Q20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R20" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1821,8 +1926,11 @@
       <c r="Q21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R21" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1874,8 +1982,11 @@
       <c r="Q22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1927,8 +2038,11 @@
       <c r="Q23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1980,8 +2094,11 @@
       <c r="Q24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2033,8 +2150,11 @@
       <c r="Q25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2086,8 +2206,11 @@
       <c r="Q26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2139,8 +2262,11 @@
       <c r="Q27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2192,8 +2318,11 @@
       <c r="Q28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2245,8 +2374,11 @@
       <c r="Q29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2298,8 +2430,11 @@
       <c r="Q30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2351,8 +2486,11 @@
       <c r="Q31" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R31" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2404,8 +2542,11 @@
       <c r="Q32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2457,8 +2598,11 @@
       <c r="Q33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2510,8 +2654,11 @@
       <c r="Q34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2563,8 +2710,11 @@
       <c r="Q35" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2616,8 +2766,11 @@
       <c r="Q36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2669,8 +2822,11 @@
       <c r="Q37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2722,8 +2878,11 @@
       <c r="Q38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2775,8 +2934,11 @@
       <c r="Q39" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2828,8 +2990,11 @@
       <c r="Q40" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2866,8 +3031,11 @@
       <c r="Q41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Added test results for Android Chrome
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947A2AE-6961-744C-98FA-1A87C48AAADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FCA8C3-D420-9B47-B41D-2F5A6DDF8988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="132">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -306,6 +306,114 @@
   </si>
   <si>
     <t>heading level 2</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>spoken by TalkBack</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>acknowledgments</t>
+  </si>
+  <si>
+    <t>afterword</t>
+  </si>
+  <si>
+    <t>appendix</t>
+  </si>
+  <si>
+    <t>backlink</t>
+  </si>
+  <si>
+    <t>bibliography reference</t>
+  </si>
+  <si>
+    <t>chapter</t>
+  </si>
+  <si>
+    <t>colophon</t>
+  </si>
+  <si>
+    <t>conclusion</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>dedication</t>
+  </si>
+  <si>
+    <t>epigraph</t>
+  </si>
+  <si>
+    <t>epilogue</t>
+  </si>
+  <si>
+    <t>errata</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>foreword</t>
+  </si>
+  <si>
+    <t>term, definition</t>
+  </si>
+  <si>
+    <t>glossary reference</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>introduction</t>
+  </si>
+  <si>
+    <t>note reference</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>title attribute ..., pagebreak</t>
+  </si>
+  <si>
+    <t>pagelist</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>preface</t>
+  </si>
+  <si>
+    <t>prologue</t>
+  </si>
+  <si>
+    <t>pullquote</t>
+  </si>
+  <si>
+    <t>qna</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>tip</t>
+  </si>
+  <si>
+    <t>table of contents</t>
   </si>
 </sst>
 </file>
@@ -400,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -420,6 +528,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,6 +538,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -773,13 +887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -802,71 +916,78 @@
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="8" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="12" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="14"/>
+      <c r="P2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="13"/>
+      <c r="Q2" s="15"/>
       <c r="R2" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S2" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -921,8 +1042,11 @@
       <c r="R3" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1101,11 @@
       <c r="R4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1033,8 +1160,11 @@
       <c r="R5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1089,8 +1219,11 @@
       <c r="R6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1145,8 +1278,11 @@
       <c r="R7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1201,8 +1337,11 @@
       <c r="R8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1257,8 +1396,11 @@
       <c r="R9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1313,8 +1455,11 @@
       <c r="R10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1369,8 +1514,11 @@
       <c r="R11" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1425,8 +1573,11 @@
       <c r="R12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1481,8 +1632,11 @@
       <c r="R13" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1537,8 +1691,11 @@
       <c r="R14" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1593,8 +1750,11 @@
       <c r="R15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1649,8 +1809,11 @@
       <c r="R16" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1705,8 +1868,11 @@
       <c r="R17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1761,8 +1927,11 @@
       <c r="R18" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1817,8 +1986,11 @@
       <c r="R19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1873,8 +2045,11 @@
       <c r="R20" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1929,8 +2104,11 @@
       <c r="R21" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1985,8 +2163,11 @@
       <c r="R22" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2041,8 +2222,11 @@
       <c r="R23" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2097,8 +2281,11 @@
       <c r="R24" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2153,8 +2340,11 @@
       <c r="R25" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2209,8 +2399,11 @@
       <c r="R26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2265,8 +2458,11 @@
       <c r="R27" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2321,8 +2517,11 @@
       <c r="R28" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2377,8 +2576,11 @@
       <c r="R29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2433,8 +2635,11 @@
       <c r="R30" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2489,8 +2694,11 @@
       <c r="R31" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2545,8 +2753,11 @@
       <c r="R32" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2601,8 +2812,11 @@
       <c r="R33" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2657,8 +2871,11 @@
       <c r="R34" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2713,8 +2930,11 @@
       <c r="R35" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2769,8 +2989,11 @@
       <c r="R36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2825,8 +3048,11 @@
       <c r="R37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2881,8 +3107,11 @@
       <c r="R38" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2937,8 +3166,11 @@
       <c r="R39" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2993,8 +3225,11 @@
       <c r="R40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3034,8 +3269,11 @@
       <c r="R41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Added the terms that are spoken by JAWS 2021 for Chrome on Windows
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FCA8C3-D420-9B47-B41D-2F5A6DDF8988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="136">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -414,12 +413,24 @@
   </si>
   <si>
     <t>table of contents</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Graphic</t>
+  </si>
+  <si>
+    <t>separater</t>
+  </si>
+  <si>
+    <t>Heading 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,7 +562,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -567,7 +578,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -609,7 +620,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,26 +653,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,23 +688,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -886,40 +863,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -935,22 +913,23 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10"/>
+      <c r="M1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="11"/>
+      <c r="S1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -960,34 +939,35 @@
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="13"/>
+      <c r="O2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1001,52 +981,55 @@
         <v>81</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1059,53 +1042,53 @@
       <c r="D4">
         <v>-1</v>
       </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
       <c r="F4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>-1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4">
-        <v>-1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4">
+        <v>-1</v>
       </c>
       <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" t="s">
-        <v>58</v>
-      </c>
       <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" t="s">
         <v>0</v>
       </c>
-      <c r="O4" t="s">
-        <v>58</v>
-      </c>
       <c r="P4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" t="s">
-        <v>58</v>
-      </c>
       <c r="R4" t="s">
         <v>58</v>
       </c>
       <c r="S4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1118,53 +1101,53 @@
       <c r="D5">
         <v>-1</v>
       </c>
-      <c r="E5">
-        <v>-1</v>
-      </c>
       <c r="F5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>-1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5">
-        <v>-1</v>
-      </c>
-      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="L5" t="s">
         <v>57</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>38</v>
       </c>
-      <c r="M5" t="s">
-        <v>58</v>
-      </c>
       <c r="N5" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="P5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" t="s">
-        <v>58</v>
-      </c>
       <c r="R5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" t="s">
         <v>90</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1177,53 +1160,53 @@
       <c r="D6">
         <v>-1</v>
       </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
       <c r="F6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>-1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6">
-        <v>-1</v>
-      </c>
-      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>-1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6" t="s">
         <v>57</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>38</v>
       </c>
-      <c r="M6" t="s">
-        <v>58</v>
-      </c>
       <c r="N6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" t="s">
         <v>2</v>
       </c>
-      <c r="O6" t="s">
-        <v>58</v>
-      </c>
       <c r="P6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" t="s">
-        <v>58</v>
-      </c>
       <c r="R6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" t="s">
         <v>90</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1236,53 +1219,53 @@
       <c r="D7">
         <v>-1</v>
       </c>
-      <c r="E7">
-        <v>-1</v>
-      </c>
       <c r="F7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>-1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7">
-        <v>-1</v>
-      </c>
-      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+      <c r="L7" t="s">
         <v>57</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
       <c r="N7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" t="s">
         <v>3</v>
       </c>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
       <c r="P7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" t="s">
-        <v>58</v>
-      </c>
       <c r="R7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" t="s">
         <v>90</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1295,53 +1278,56 @@
       <c r="D8">
         <v>-1</v>
       </c>
-      <c r="E8">
-        <v>-1</v>
+      <c r="E8" t="s">
+        <v>132</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>-1</v>
-      </c>
-      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>-1</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
       </c>
-      <c r="J8">
-        <v>-1</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8" t="s">
         <v>63</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>39</v>
       </c>
-      <c r="M8" t="s">
-        <v>58</v>
-      </c>
       <c r="N8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" t="s">
         <v>4</v>
       </c>
-      <c r="O8" t="s">
-        <v>58</v>
-      </c>
       <c r="P8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" t="s">
         <v>63</v>
       </c>
-      <c r="Q8" t="s">
-        <v>58</v>
-      </c>
       <c r="R8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" t="s">
         <v>63</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1354,53 +1340,53 @@
       <c r="D9">
         <v>-1</v>
       </c>
-      <c r="E9">
-        <v>-1</v>
-      </c>
       <c r="F9">
         <v>-1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H9">
-        <v>-1</v>
-      </c>
-      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+      <c r="J9" t="s">
         <v>67</v>
       </c>
-      <c r="J9">
-        <v>-1</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9" t="s">
         <v>57</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>38</v>
       </c>
-      <c r="M9" t="s">
-        <v>58</v>
-      </c>
       <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
         <v>5</v>
       </c>
-      <c r="O9" t="s">
-        <v>58</v>
-      </c>
       <c r="P9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" t="s">
         <v>57</v>
       </c>
-      <c r="Q9" t="s">
-        <v>58</v>
-      </c>
       <c r="R9" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" t="s">
         <v>90</v>
       </c>
-      <c r="S9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1413,53 +1399,56 @@
       <c r="D10">
         <v>-1</v>
       </c>
-      <c r="E10">
-        <v>-1</v>
+      <c r="E10" t="s">
+        <v>132</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>-1</v>
-      </c>
-      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>-1</v>
+      </c>
+      <c r="J10" t="s">
         <v>63</v>
       </c>
-      <c r="J10">
-        <v>-1</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>-1</v>
+      </c>
+      <c r="L10" t="s">
         <v>63</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>39</v>
       </c>
-      <c r="M10" t="s">
-        <v>58</v>
-      </c>
       <c r="N10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" t="s">
         <v>6</v>
       </c>
-      <c r="O10" t="s">
-        <v>58</v>
-      </c>
       <c r="P10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" t="s">
         <v>63</v>
       </c>
-      <c r="Q10" t="s">
-        <v>58</v>
-      </c>
       <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
         <v>63</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1472,53 +1461,53 @@
       <c r="D11">
         <v>-1</v>
       </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
       <c r="F11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>-1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11">
-        <v>-1</v>
-      </c>
-      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>-1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+      <c r="L11" t="s">
         <v>57</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>38</v>
       </c>
-      <c r="M11" t="s">
-        <v>58</v>
-      </c>
       <c r="N11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" t="s">
         <v>7</v>
       </c>
-      <c r="O11" t="s">
-        <v>58</v>
-      </c>
       <c r="P11" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q11" t="s">
         <v>57</v>
       </c>
-      <c r="Q11" t="s">
-        <v>58</v>
-      </c>
-      <c r="R11" s="6" t="s">
+      <c r="R11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1531,53 +1520,53 @@
       <c r="D12">
         <v>-1</v>
       </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
       <c r="F12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>-1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12">
-        <v>-1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>-1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12">
+        <v>-1</v>
       </c>
       <c r="L12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" t="s">
         <v>37</v>
       </c>
-      <c r="M12" t="s">
-        <v>58</v>
-      </c>
       <c r="N12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" t="s">
         <v>8</v>
       </c>
-      <c r="O12" t="s">
-        <v>58</v>
-      </c>
       <c r="P12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" t="s">
-        <v>58</v>
-      </c>
       <c r="R12" t="s">
         <v>58</v>
       </c>
       <c r="S12" t="s">
+        <v>58</v>
+      </c>
+      <c r="T12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1590,53 +1579,53 @@
       <c r="D13">
         <v>-1</v>
       </c>
-      <c r="E13">
-        <v>-1</v>
-      </c>
       <c r="F13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>-1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13">
-        <v>-1</v>
-      </c>
-      <c r="K13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>-1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13">
+        <v>-1</v>
+      </c>
+      <c r="L13" t="s">
         <v>57</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>38</v>
       </c>
-      <c r="M13" t="s">
-        <v>58</v>
-      </c>
       <c r="N13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" t="s">
         <v>9</v>
       </c>
-      <c r="O13" t="s">
-        <v>58</v>
-      </c>
       <c r="P13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" t="s">
         <v>57</v>
       </c>
-      <c r="Q13" t="s">
-        <v>58</v>
-      </c>
-      <c r="R13" s="6" t="s">
+      <c r="R13" t="s">
+        <v>58</v>
+      </c>
+      <c r="S13" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1649,53 +1638,56 @@
       <c r="D14">
         <v>-1</v>
       </c>
-      <c r="E14">
-        <v>-1</v>
+      <c r="E14" t="s">
+        <v>133</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>-1</v>
-      </c>
-      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>-1</v>
+      </c>
+      <c r="J14" t="s">
         <v>65</v>
       </c>
-      <c r="J14">
-        <v>-1</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="K14">
+        <v>-1</v>
+      </c>
+      <c r="L14" t="s">
         <v>65</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>41</v>
       </c>
-      <c r="M14" t="s">
-        <v>58</v>
-      </c>
       <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
         <v>10</v>
       </c>
-      <c r="O14" t="s">
-        <v>58</v>
-      </c>
       <c r="P14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" t="s">
         <v>65</v>
       </c>
-      <c r="Q14" t="s">
-        <v>58</v>
-      </c>
       <c r="R14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S14" t="s">
         <v>91</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1708,53 +1700,53 @@
       <c r="D15">
         <v>-1</v>
       </c>
-      <c r="E15">
-        <v>-1</v>
-      </c>
       <c r="F15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>-1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15">
-        <v>-1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>-1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15">
+        <v>-1</v>
       </c>
       <c r="L15" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" t="s">
         <v>37</v>
       </c>
-      <c r="M15" t="s">
-        <v>58</v>
-      </c>
       <c r="N15" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" t="s">
         <v>11</v>
       </c>
-      <c r="O15" t="s">
-        <v>58</v>
-      </c>
       <c r="P15" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" t="s">
         <v>69</v>
       </c>
-      <c r="Q15" t="s">
-        <v>58</v>
-      </c>
       <c r="R15" t="s">
         <v>58</v>
       </c>
       <c r="S15" t="s">
+        <v>58</v>
+      </c>
+      <c r="T15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1767,53 +1759,53 @@
       <c r="D16">
         <v>-1</v>
       </c>
-      <c r="E16">
-        <v>-1</v>
-      </c>
       <c r="F16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>-1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16">
-        <v>-1</v>
-      </c>
-      <c r="K16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>-1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+      <c r="L16" t="s">
         <v>64</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>38</v>
       </c>
-      <c r="M16" t="s">
-        <v>58</v>
-      </c>
       <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
         <v>12</v>
       </c>
-      <c r="O16" t="s">
-        <v>58</v>
-      </c>
       <c r="P16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q16" t="s">
         <v>57</v>
       </c>
-      <c r="Q16" t="s">
-        <v>58</v>
-      </c>
-      <c r="R16" s="6" t="s">
+      <c r="R16" t="s">
+        <v>58</v>
+      </c>
+      <c r="S16" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1826,53 +1818,53 @@
       <c r="D17">
         <v>-1</v>
       </c>
-      <c r="E17">
-        <v>-1</v>
-      </c>
       <c r="F17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>-1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17">
-        <v>-1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>-1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17">
+        <v>-1</v>
       </c>
       <c r="L17" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" t="s">
         <v>37</v>
       </c>
-      <c r="M17" t="s">
-        <v>58</v>
-      </c>
       <c r="N17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" t="s">
         <v>13</v>
       </c>
-      <c r="O17" t="s">
-        <v>58</v>
-      </c>
       <c r="P17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q17" t="s">
         <v>69</v>
       </c>
-      <c r="Q17" t="s">
-        <v>58</v>
-      </c>
       <c r="R17" t="s">
         <v>58</v>
       </c>
       <c r="S17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1885,53 +1877,53 @@
       <c r="D18">
         <v>-1</v>
       </c>
-      <c r="E18">
-        <v>-1</v>
-      </c>
       <c r="F18">
         <v>-1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H18">
-        <v>-1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18">
-        <v>-1</v>
-      </c>
-      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>-1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18">
+        <v>-1</v>
+      </c>
+      <c r="L18" t="s">
         <v>57</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>38</v>
       </c>
-      <c r="M18" t="s">
-        <v>58</v>
-      </c>
       <c r="N18" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" t="s">
         <v>14</v>
       </c>
-      <c r="O18" t="s">
-        <v>58</v>
-      </c>
       <c r="P18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" t="s">
         <v>57</v>
       </c>
-      <c r="Q18" t="s">
-        <v>58</v>
-      </c>
-      <c r="R18" s="6" t="s">
+      <c r="R18" t="s">
+        <v>58</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1944,53 +1936,53 @@
       <c r="D19">
         <v>-1</v>
       </c>
-      <c r="E19">
-        <v>-1</v>
-      </c>
       <c r="F19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19">
-        <v>-1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19">
-        <v>-1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>-1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19">
+        <v>-1</v>
       </c>
       <c r="L19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19" t="s">
         <v>37</v>
       </c>
-      <c r="M19" t="s">
-        <v>58</v>
-      </c>
       <c r="N19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O19" t="s">
         <v>15</v>
       </c>
-      <c r="O19" t="s">
-        <v>58</v>
-      </c>
       <c r="P19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q19" t="s">
         <v>69</v>
       </c>
-      <c r="Q19" t="s">
-        <v>58</v>
-      </c>
       <c r="R19" t="s">
         <v>58</v>
       </c>
       <c r="S19" t="s">
+        <v>58</v>
+      </c>
+      <c r="T19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2003,53 +1995,53 @@
       <c r="D20">
         <v>-1</v>
       </c>
-      <c r="E20">
-        <v>-1</v>
-      </c>
       <c r="F20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>-1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20">
-        <v>-1</v>
-      </c>
-      <c r="K20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>-1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20">
+        <v>-1</v>
+      </c>
+      <c r="L20" t="s">
         <v>57</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>38</v>
       </c>
-      <c r="M20" t="s">
-        <v>58</v>
-      </c>
       <c r="N20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O20" t="s">
         <v>16</v>
       </c>
-      <c r="O20" t="s">
-        <v>58</v>
-      </c>
       <c r="P20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q20" t="s">
         <v>57</v>
       </c>
-      <c r="Q20" t="s">
-        <v>58</v>
-      </c>
-      <c r="R20" s="6" t="s">
+      <c r="R20" t="s">
+        <v>58</v>
+      </c>
+      <c r="S20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2062,53 +2054,53 @@
       <c r="D21">
         <v>-1</v>
       </c>
-      <c r="E21">
-        <v>-1</v>
-      </c>
       <c r="F21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>-1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21">
-        <v>-1</v>
-      </c>
-      <c r="K21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>-1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21">
+        <v>-1</v>
+      </c>
+      <c r="L21" t="s">
         <v>57</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>38</v>
       </c>
-      <c r="M21" t="s">
-        <v>58</v>
-      </c>
       <c r="N21" t="s">
+        <v>58</v>
+      </c>
+      <c r="O21" t="s">
         <v>17</v>
       </c>
-      <c r="O21" t="s">
-        <v>58</v>
-      </c>
       <c r="P21" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q21" t="s">
         <v>57</v>
       </c>
-      <c r="Q21" t="s">
-        <v>58</v>
-      </c>
-      <c r="R21" s="6" t="s">
+      <c r="R21" t="s">
+        <v>58</v>
+      </c>
+      <c r="S21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2121,53 +2113,53 @@
       <c r="D22">
         <v>-1</v>
       </c>
-      <c r="E22">
-        <v>-1</v>
-      </c>
       <c r="F22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>-1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22">
-        <v>-1</v>
-      </c>
-      <c r="K22" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>-1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22">
+        <v>-1</v>
       </c>
       <c r="L22" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" t="s">
-        <v>58</v>
-      </c>
       <c r="N22" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" t="s">
         <v>18</v>
       </c>
-      <c r="O22" t="s">
-        <v>58</v>
-      </c>
       <c r="P22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q22" t="s">
         <v>69</v>
       </c>
-      <c r="Q22" t="s">
-        <v>58</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S22" t="s">
+      <c r="R22" t="s">
+        <v>58</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="T22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2180,9 +2172,6 @@
       <c r="D23">
         <v>-1</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
       <c r="F23">
         <v>1</v>
       </c>
@@ -2190,43 +2179,46 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>-1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>-1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
         <v>59</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>37</v>
       </c>
-      <c r="M23" t="s">
-        <v>58</v>
-      </c>
       <c r="N23" t="s">
+        <v>58</v>
+      </c>
+      <c r="O23" t="s">
         <v>19</v>
       </c>
-      <c r="O23" t="s">
-        <v>58</v>
-      </c>
       <c r="P23" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q23" t="s">
         <v>59</v>
       </c>
-      <c r="Q23" t="s">
-        <v>58</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="R23" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="T23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2239,53 +2231,53 @@
       <c r="D24">
         <v>-1</v>
       </c>
-      <c r="E24">
-        <v>-1</v>
-      </c>
       <c r="F24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>-1</v>
-      </c>
-      <c r="I24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J24">
-        <v>-1</v>
-      </c>
-      <c r="K24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>-1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24">
+        <v>-1</v>
+      </c>
+      <c r="L24" t="s">
         <v>57</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>38</v>
       </c>
-      <c r="M24" t="s">
-        <v>58</v>
-      </c>
       <c r="N24" t="s">
+        <v>58</v>
+      </c>
+      <c r="O24" t="s">
         <v>20</v>
       </c>
-      <c r="O24" t="s">
-        <v>58</v>
-      </c>
       <c r="P24" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q24" t="s">
         <v>57</v>
       </c>
-      <c r="Q24" t="s">
-        <v>58</v>
-      </c>
-      <c r="R24" s="6" t="s">
+      <c r="R24" t="s">
+        <v>58</v>
+      </c>
+      <c r="S24" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2298,53 +2290,53 @@
       <c r="D25">
         <v>-1</v>
       </c>
-      <c r="E25">
-        <v>-1</v>
-      </c>
       <c r="F25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>-1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>58</v>
-      </c>
-      <c r="J25">
-        <v>-1</v>
-      </c>
-      <c r="K25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>-1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25">
+        <v>-1</v>
+      </c>
+      <c r="L25" t="s">
         <v>57</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>38</v>
       </c>
-      <c r="M25" t="s">
-        <v>58</v>
-      </c>
       <c r="N25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="O25" t="s">
-        <v>58</v>
-      </c>
       <c r="P25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q25" t="s">
         <v>57</v>
       </c>
-      <c r="Q25" t="s">
-        <v>58</v>
-      </c>
-      <c r="R25" s="6" t="s">
+      <c r="R25" t="s">
+        <v>58</v>
+      </c>
+      <c r="S25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2357,53 +2349,56 @@
       <c r="D26">
         <v>-1</v>
       </c>
-      <c r="E26">
-        <v>-1</v>
+      <c r="E26" t="s">
+        <v>132</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
-        <v>-1</v>
-      </c>
-      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>-1</v>
+      </c>
+      <c r="J26" t="s">
         <v>63</v>
       </c>
-      <c r="J26">
-        <v>-1</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="K26">
+        <v>-1</v>
+      </c>
+      <c r="L26" t="s">
         <v>63</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>39</v>
       </c>
-      <c r="M26" t="s">
-        <v>58</v>
-      </c>
       <c r="N26" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" t="s">
         <v>22</v>
       </c>
-      <c r="O26" t="s">
-        <v>58</v>
-      </c>
       <c r="P26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" t="s">
         <v>63</v>
       </c>
-      <c r="Q26" t="s">
-        <v>58</v>
-      </c>
       <c r="R26" t="s">
+        <v>58</v>
+      </c>
+      <c r="S26" t="s">
         <v>63</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2416,53 +2411,53 @@
       <c r="D27">
         <v>-1</v>
       </c>
-      <c r="E27">
-        <v>-1</v>
-      </c>
       <c r="F27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
-        <v>-1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>58</v>
-      </c>
-      <c r="J27">
-        <v>-1</v>
-      </c>
-      <c r="K27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>-1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27">
+        <v>-1</v>
+      </c>
+      <c r="L27" t="s">
         <v>57</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>42</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>51</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>23</v>
       </c>
-      <c r="O27" t="s">
-        <v>58</v>
-      </c>
       <c r="P27" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q27" t="s">
         <v>70</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>51</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>92</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2475,53 +2470,53 @@
       <c r="D28">
         <v>-1</v>
       </c>
-      <c r="E28">
-        <v>-1</v>
-      </c>
       <c r="F28">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>-1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>58</v>
-      </c>
-      <c r="J28">
-        <v>-1</v>
-      </c>
-      <c r="K28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>-1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28">
+        <v>-1</v>
+      </c>
+      <c r="L28" t="s">
         <v>57</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>38</v>
       </c>
-      <c r="M28" t="s">
-        <v>58</v>
-      </c>
       <c r="N28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O28" t="s">
         <v>24</v>
       </c>
-      <c r="O28" t="s">
-        <v>58</v>
-      </c>
       <c r="P28" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q28" t="s">
         <v>57</v>
       </c>
-      <c r="Q28" t="s">
-        <v>58</v>
-      </c>
-      <c r="R28" s="6" t="s">
+      <c r="R28" t="s">
+        <v>58</v>
+      </c>
+      <c r="S28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2534,53 +2529,56 @@
       <c r="D29">
         <v>-1</v>
       </c>
-      <c r="E29">
-        <v>-1</v>
+      <c r="E29" t="s">
+        <v>63</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>-1</v>
-      </c>
-      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>-1</v>
+      </c>
+      <c r="J29" t="s">
         <v>63</v>
       </c>
-      <c r="J29">
-        <v>-1</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="K29">
+        <v>-1</v>
+      </c>
+      <c r="L29" t="s">
         <v>63</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>39</v>
       </c>
-      <c r="M29" t="s">
-        <v>58</v>
-      </c>
       <c r="N29" t="s">
+        <v>58</v>
+      </c>
+      <c r="O29" t="s">
         <v>25</v>
       </c>
-      <c r="O29" t="s">
-        <v>58</v>
-      </c>
       <c r="P29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q29" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" t="s">
-        <v>58</v>
-      </c>
       <c r="R29" t="s">
+        <v>58</v>
+      </c>
+      <c r="S29" t="s">
         <v>63</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2593,53 +2591,56 @@
       <c r="D30">
         <v>-1</v>
       </c>
-      <c r="E30">
-        <v>-1</v>
+      <c r="E30" t="s">
+        <v>66</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>-1</v>
-      </c>
-      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>-1</v>
+      </c>
+      <c r="J30" t="s">
         <v>66</v>
       </c>
-      <c r="J30">
-        <v>-1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>58</v>
+      <c r="K30">
+        <v>-1</v>
       </c>
       <c r="L30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" t="s">
         <v>43</v>
       </c>
-      <c r="M30" t="s">
-        <v>58</v>
-      </c>
       <c r="N30" t="s">
+        <v>58</v>
+      </c>
+      <c r="O30" t="s">
         <v>26</v>
       </c>
-      <c r="O30" t="s">
-        <v>58</v>
-      </c>
       <c r="P30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q30" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" t="s">
-        <v>58</v>
-      </c>
       <c r="R30" t="s">
+        <v>58</v>
+      </c>
+      <c r="S30" t="s">
         <v>93</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2652,53 +2653,56 @@
       <c r="D31">
         <v>-1</v>
       </c>
-      <c r="E31">
-        <v>-1</v>
+      <c r="E31" t="s">
+        <v>134</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>-1</v>
-      </c>
-      <c r="I31" t="s">
-        <v>58</v>
-      </c>
-      <c r="J31">
-        <v>-1</v>
-      </c>
-      <c r="K31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>-1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31">
+        <v>-1</v>
+      </c>
+      <c r="L31" t="s">
         <v>62</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>44</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>48</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>27</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>48</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>62</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>52</v>
       </c>
-      <c r="R31" s="7" t="s">
+      <c r="S31" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2711,53 +2715,53 @@
       <c r="D32">
         <v>-1</v>
       </c>
-      <c r="E32">
-        <v>-1</v>
-      </c>
       <c r="F32">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>-1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>58</v>
-      </c>
-      <c r="J32">
-        <v>-1</v>
-      </c>
-      <c r="K32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>-1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32">
+        <v>-1</v>
+      </c>
+      <c r="L32" t="s">
         <v>57</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>42</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>51</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>28</v>
       </c>
-      <c r="O32" t="s">
-        <v>58</v>
-      </c>
       <c r="P32" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q32" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>51</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>92</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2770,53 +2774,53 @@
       <c r="D33">
         <v>-1</v>
       </c>
-      <c r="E33">
-        <v>-1</v>
-      </c>
       <c r="F33">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>-1</v>
-      </c>
-      <c r="I33" t="s">
-        <v>58</v>
-      </c>
-      <c r="J33">
-        <v>-1</v>
-      </c>
-      <c r="K33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>-1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33">
+        <v>-1</v>
+      </c>
+      <c r="L33" t="s">
         <v>57</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>38</v>
       </c>
-      <c r="M33" t="s">
-        <v>58</v>
-      </c>
       <c r="N33" t="s">
+        <v>58</v>
+      </c>
+      <c r="O33" t="s">
         <v>29</v>
       </c>
-      <c r="O33" t="s">
-        <v>58</v>
-      </c>
       <c r="P33" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q33" t="s">
         <v>57</v>
       </c>
-      <c r="Q33" t="s">
-        <v>58</v>
-      </c>
-      <c r="R33" s="6" t="s">
+      <c r="R33" t="s">
+        <v>58</v>
+      </c>
+      <c r="S33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2829,53 +2833,53 @@
       <c r="D34">
         <v>-1</v>
       </c>
-      <c r="E34">
-        <v>-1</v>
-      </c>
       <c r="F34">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>-1</v>
-      </c>
-      <c r="I34" t="s">
-        <v>58</v>
-      </c>
-      <c r="J34">
-        <v>-1</v>
-      </c>
-      <c r="K34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>-1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34">
+        <v>-1</v>
+      </c>
+      <c r="L34" t="s">
         <v>57</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>38</v>
       </c>
-      <c r="M34" t="s">
-        <v>58</v>
-      </c>
       <c r="N34" t="s">
+        <v>58</v>
+      </c>
+      <c r="O34" t="s">
         <v>30</v>
       </c>
-      <c r="O34" t="s">
-        <v>58</v>
-      </c>
       <c r="P34" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q34" t="s">
         <v>57</v>
       </c>
-      <c r="Q34" t="s">
-        <v>58</v>
-      </c>
-      <c r="R34" s="6" t="s">
+      <c r="R34" t="s">
+        <v>58</v>
+      </c>
+      <c r="S34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2888,53 +2892,53 @@
       <c r="D35">
         <v>-1</v>
       </c>
-      <c r="E35">
-        <v>-1</v>
-      </c>
       <c r="F35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
-        <v>-1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>58</v>
-      </c>
-      <c r="J35">
-        <v>-1</v>
-      </c>
-      <c r="K35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>-1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35">
+        <v>-1</v>
+      </c>
+      <c r="L35" t="s">
         <v>57</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>38</v>
       </c>
-      <c r="M35" t="s">
-        <v>58</v>
-      </c>
       <c r="N35" t="s">
+        <v>58</v>
+      </c>
+      <c r="O35" t="s">
         <v>31</v>
       </c>
-      <c r="O35" t="s">
-        <v>58</v>
-      </c>
       <c r="P35" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q35" t="s">
         <v>57</v>
       </c>
-      <c r="Q35" t="s">
-        <v>58</v>
-      </c>
-      <c r="R35" s="6" t="s">
+      <c r="R35" t="s">
+        <v>58</v>
+      </c>
+      <c r="S35" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2947,53 +2951,53 @@
       <c r="D36">
         <v>-1</v>
       </c>
-      <c r="E36">
-        <v>-1</v>
-      </c>
       <c r="F36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>-1</v>
-      </c>
-      <c r="I36" t="s">
-        <v>58</v>
-      </c>
-      <c r="J36">
-        <v>-1</v>
-      </c>
-      <c r="K36" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>-1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>58</v>
+      </c>
+      <c r="K36">
+        <v>-1</v>
       </c>
       <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" t="s">
         <v>37</v>
       </c>
-      <c r="M36" t="s">
-        <v>58</v>
-      </c>
       <c r="N36" t="s">
+        <v>58</v>
+      </c>
+      <c r="O36" t="s">
         <v>32</v>
       </c>
-      <c r="O36" t="s">
-        <v>58</v>
-      </c>
       <c r="P36" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q36" t="s">
         <v>69</v>
       </c>
-      <c r="Q36" t="s">
-        <v>58</v>
-      </c>
       <c r="R36" t="s">
         <v>58</v>
       </c>
       <c r="S36" t="s">
+        <v>58</v>
+      </c>
+      <c r="T36" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3006,53 +3010,53 @@
       <c r="D37">
         <v>-1</v>
       </c>
-      <c r="E37">
-        <v>-1</v>
-      </c>
       <c r="F37">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>-1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>58</v>
-      </c>
-      <c r="J37">
-        <v>-1</v>
-      </c>
-      <c r="K37" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>-1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37">
+        <v>-1</v>
       </c>
       <c r="L37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M37" t="s">
         <v>37</v>
       </c>
-      <c r="M37" t="s">
-        <v>58</v>
-      </c>
       <c r="N37" t="s">
+        <v>58</v>
+      </c>
+      <c r="O37" t="s">
         <v>33</v>
       </c>
-      <c r="O37" t="s">
-        <v>58</v>
-      </c>
       <c r="P37" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q37" t="s">
         <v>69</v>
       </c>
-      <c r="Q37" t="s">
-        <v>58</v>
-      </c>
       <c r="R37" t="s">
         <v>58</v>
       </c>
       <c r="S37" t="s">
+        <v>58</v>
+      </c>
+      <c r="T37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3065,53 +3069,56 @@
       <c r="D38">
         <v>-1</v>
       </c>
-      <c r="E38">
-        <v>-1</v>
+      <c r="E38" t="s">
+        <v>135</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>-1</v>
-      </c>
-      <c r="I38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>-1</v>
+      </c>
+      <c r="J38" t="s">
         <v>61</v>
       </c>
-      <c r="J38">
-        <v>-1</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="K38">
+        <v>-1</v>
+      </c>
+      <c r="L38" t="s">
         <v>68</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>40</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>50</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>34</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>49</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>68</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>49</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>95</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3124,53 +3131,56 @@
       <c r="D39">
         <v>-1</v>
       </c>
-      <c r="E39">
-        <v>-1</v>
+      <c r="E39" t="s">
+        <v>66</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
-        <v>-1</v>
-      </c>
-      <c r="I39" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>-1</v>
+      </c>
+      <c r="J39" t="s">
         <v>66</v>
       </c>
-      <c r="J39">
-        <v>-1</v>
-      </c>
-      <c r="K39" t="s">
-        <v>58</v>
+      <c r="K39">
+        <v>-1</v>
       </c>
       <c r="L39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" t="s">
         <v>43</v>
       </c>
-      <c r="M39" t="s">
-        <v>58</v>
-      </c>
       <c r="N39" t="s">
+        <v>58</v>
+      </c>
+      <c r="O39" t="s">
         <v>35</v>
       </c>
-      <c r="O39" t="s">
-        <v>58</v>
-      </c>
       <c r="P39" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q39" t="s">
         <v>66</v>
       </c>
-      <c r="Q39" t="s">
-        <v>58</v>
-      </c>
       <c r="R39" t="s">
+        <v>58</v>
+      </c>
+      <c r="S39" t="s">
         <v>93</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3183,119 +3193,119 @@
       <c r="D40">
         <v>-1</v>
       </c>
-      <c r="E40">
-        <v>-1</v>
-      </c>
       <c r="F40">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>-1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>58</v>
-      </c>
-      <c r="J40">
-        <v>-1</v>
-      </c>
-      <c r="K40" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>-1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>58</v>
+      </c>
+      <c r="K40">
+        <v>-1</v>
+      </c>
+      <c r="L40" t="s">
         <v>60</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>42</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>51</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>36</v>
       </c>
-      <c r="O40" t="s">
-        <v>58</v>
-      </c>
       <c r="P40" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q40" t="s">
         <v>70</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>51</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>92</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
       <c r="H41">
-        <v>-1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>58</v>
-      </c>
-      <c r="J41">
-        <v>-1</v>
-      </c>
-      <c r="K41" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>-1</v>
+      </c>
+      <c r="J41" t="s">
+        <v>58</v>
+      </c>
+      <c r="K41">
+        <v>-1</v>
       </c>
       <c r="L41" t="s">
+        <v>58</v>
+      </c>
+      <c r="M41" t="s">
         <v>47</v>
       </c>
-      <c r="M41" t="s">
-        <v>58</v>
-      </c>
       <c r="N41" t="s">
+        <v>58</v>
+      </c>
+      <c r="O41" t="s">
         <v>46</v>
       </c>
-      <c r="O41" t="s">
-        <v>58</v>
-      </c>
       <c r="P41" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q41" t="s">
         <v>69</v>
       </c>
-      <c r="Q41" t="s">
-        <v>58</v>
-      </c>
       <c r="R41" t="s">
         <v>58</v>
       </c>
       <c r="S41" t="s">
+        <v>58</v>
+      </c>
+      <c r="T41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>54</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>53</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>55</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added spoken terms by NVDA for Chrome on Windows
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="137">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>Heading 2</t>
+  </si>
+  <si>
+    <t>Sseparater</t>
   </si>
 </sst>
 </file>
@@ -864,13 +867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,25 +882,25 @@
     <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.36328125" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -914,22 +917,23 @@
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
       <c r="R1" s="11"/>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="11"/>
+      <c r="T1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -940,34 +944,35 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="13"/>
+      <c r="P2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -987,49 +992,52 @@
         <v>82</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>88</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1045,50 +1053,50 @@
       <c r="F4">
         <v>-1</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>-1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4">
-        <v>-1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4">
+        <v>-1</v>
       </c>
       <c r="M4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
         <v>37</v>
       </c>
-      <c r="N4" t="s">
-        <v>58</v>
-      </c>
       <c r="O4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" t="s">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>58</v>
-      </c>
       <c r="Q4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" t="s">
         <v>69</v>
       </c>
-      <c r="R4" t="s">
-        <v>58</v>
-      </c>
       <c r="S4" t="s">
         <v>58</v>
       </c>
       <c r="T4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1104,50 +1112,53 @@
       <c r="F5">
         <v>-1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
+      <c r="G5" t="s">
+        <v>57</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>-1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5">
-        <v>-1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5">
+        <v>-1</v>
       </c>
       <c r="M5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" t="s">
         <v>38</v>
       </c>
-      <c r="N5" t="s">
-        <v>58</v>
-      </c>
       <c r="O5" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S5" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" t="s">
         <v>90</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1163,50 +1174,53 @@
       <c r="F6">
         <v>-1</v>
       </c>
-      <c r="G6">
-        <v>1</v>
+      <c r="G6" t="s">
+        <v>57</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>-1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6">
-        <v>-1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>-1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6">
+        <v>-1</v>
       </c>
       <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" t="s">
         <v>38</v>
       </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
       <c r="O6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" t="s">
         <v>2</v>
       </c>
-      <c r="P6" t="s">
-        <v>58</v>
-      </c>
       <c r="Q6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S6" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" t="s">
         <v>90</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1222,50 +1236,53 @@
       <c r="F7">
         <v>-1</v>
       </c>
-      <c r="G7">
-        <v>1</v>
+      <c r="G7" t="s">
+        <v>57</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>-1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7">
-        <v>-1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
       </c>
       <c r="M7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" t="s">
         <v>38</v>
       </c>
-      <c r="N7" t="s">
-        <v>58</v>
-      </c>
       <c r="O7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="P7" t="s">
-        <v>58</v>
-      </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S7" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" t="s">
         <v>90</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1284,50 +1301,53 @@
       <c r="F8">
         <v>-1</v>
       </c>
-      <c r="G8">
-        <v>1</v>
+      <c r="G8" t="s">
+        <v>63</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>-1</v>
-      </c>
-      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8" t="s">
         <v>63</v>
       </c>
-      <c r="K8">
-        <v>-1</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8" t="s">
         <v>63</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>39</v>
       </c>
-      <c r="N8" t="s">
-        <v>58</v>
-      </c>
       <c r="O8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" t="s">
         <v>4</v>
       </c>
-      <c r="P8" t="s">
-        <v>58</v>
-      </c>
       <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s">
         <v>63</v>
       </c>
-      <c r="R8" t="s">
-        <v>58</v>
-      </c>
       <c r="S8" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" t="s">
         <v>63</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1343,50 +1363,53 @@
       <c r="F9">
         <v>-1</v>
       </c>
-      <c r="G9">
-        <v>-1</v>
+      <c r="G9" t="s">
+        <v>57</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I9">
-        <v>-1</v>
-      </c>
-      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>-1</v>
+      </c>
+      <c r="K9" t="s">
         <v>67</v>
       </c>
-      <c r="K9">
-        <v>-1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>57</v>
+      <c r="L9">
+        <v>-1</v>
       </c>
       <c r="M9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" t="s">
         <v>38</v>
       </c>
-      <c r="N9" t="s">
-        <v>58</v>
-      </c>
       <c r="O9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" t="s">
         <v>5</v>
       </c>
-      <c r="P9" t="s">
-        <v>58</v>
-      </c>
       <c r="Q9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" t="s">
         <v>90</v>
       </c>
-      <c r="T9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1405,50 +1428,53 @@
       <c r="F10">
         <v>-1</v>
       </c>
-      <c r="G10">
-        <v>1</v>
+      <c r="G10" t="s">
+        <v>63</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>-1</v>
-      </c>
-      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
+      <c r="K10" t="s">
         <v>63</v>
       </c>
-      <c r="K10">
-        <v>-1</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10" t="s">
         <v>63</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>39</v>
       </c>
-      <c r="N10" t="s">
-        <v>58</v>
-      </c>
       <c r="O10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" t="s">
         <v>6</v>
       </c>
-      <c r="P10" t="s">
-        <v>58</v>
-      </c>
       <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" t="s">
         <v>63</v>
       </c>
-      <c r="R10" t="s">
-        <v>58</v>
-      </c>
       <c r="S10" t="s">
+        <v>58</v>
+      </c>
+      <c r="T10" t="s">
         <v>63</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1464,50 +1490,50 @@
       <c r="F11">
         <v>-1</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11">
-        <v>-1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11">
-        <v>-1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>-1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11">
+        <v>-1</v>
       </c>
       <c r="M11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" t="s">
         <v>38</v>
       </c>
-      <c r="N11" t="s">
-        <v>58</v>
-      </c>
       <c r="O11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" t="s">
         <v>7</v>
       </c>
-      <c r="P11" t="s">
-        <v>58</v>
-      </c>
       <c r="Q11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R11" t="s">
-        <v>58</v>
-      </c>
-      <c r="S11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S11" t="s">
+        <v>58</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1523,50 +1549,50 @@
       <c r="F12">
         <v>-1</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>-1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12">
-        <v>-1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>-1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
       </c>
       <c r="M12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N12" t="s">
         <v>37</v>
       </c>
-      <c r="N12" t="s">
-        <v>58</v>
-      </c>
       <c r="O12" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" t="s">
         <v>8</v>
       </c>
-      <c r="P12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" t="s">
         <v>69</v>
       </c>
-      <c r="R12" t="s">
-        <v>58</v>
-      </c>
       <c r="S12" t="s">
         <v>58</v>
       </c>
       <c r="T12" t="s">
+        <v>58</v>
+      </c>
+      <c r="U12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1582,50 +1608,50 @@
       <c r="F13">
         <v>-1</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <v>-1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13">
-        <v>-1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13">
+        <v>-1</v>
       </c>
       <c r="M13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" t="s">
         <v>38</v>
       </c>
-      <c r="N13" t="s">
-        <v>58</v>
-      </c>
       <c r="O13" t="s">
+        <v>58</v>
+      </c>
+      <c r="P13" t="s">
         <v>9</v>
       </c>
-      <c r="P13" t="s">
-        <v>58</v>
-      </c>
       <c r="Q13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S13" t="s">
+        <v>58</v>
+      </c>
+      <c r="T13" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1644,50 +1670,50 @@
       <c r="F14">
         <v>-1</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>-1</v>
-      </c>
-      <c r="J14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>-1</v>
+      </c>
+      <c r="K14" t="s">
         <v>65</v>
       </c>
-      <c r="K14">
-        <v>-1</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="L14">
+        <v>-1</v>
+      </c>
+      <c r="M14" t="s">
         <v>65</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>41</v>
       </c>
-      <c r="N14" t="s">
-        <v>58</v>
-      </c>
       <c r="O14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" t="s">
         <v>10</v>
       </c>
-      <c r="P14" t="s">
-        <v>58</v>
-      </c>
       <c r="Q14" t="s">
+        <v>58</v>
+      </c>
+      <c r="R14" t="s">
         <v>65</v>
       </c>
-      <c r="R14" t="s">
-        <v>58</v>
-      </c>
       <c r="S14" t="s">
+        <v>58</v>
+      </c>
+      <c r="T14" t="s">
         <v>91</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1703,50 +1729,50 @@
       <c r="F15">
         <v>-1</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <v>-1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15">
-        <v>-1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>-1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15">
+        <v>-1</v>
       </c>
       <c r="M15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" t="s">
         <v>37</v>
       </c>
-      <c r="N15" t="s">
-        <v>58</v>
-      </c>
       <c r="O15" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" t="s">
         <v>11</v>
       </c>
-      <c r="P15" t="s">
-        <v>58</v>
-      </c>
       <c r="Q15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R15" t="s">
         <v>69</v>
       </c>
-      <c r="R15" t="s">
-        <v>58</v>
-      </c>
       <c r="S15" t="s">
         <v>58</v>
       </c>
       <c r="T15" t="s">
+        <v>58</v>
+      </c>
+      <c r="U15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1762,50 +1788,50 @@
       <c r="F16">
         <v>-1</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
-        <v>-1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16">
-        <v>-1</v>
-      </c>
-      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>-1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16">
+        <v>-1</v>
+      </c>
+      <c r="M16" t="s">
         <v>64</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>38</v>
       </c>
-      <c r="N16" t="s">
-        <v>58</v>
-      </c>
       <c r="O16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P16" t="s">
         <v>12</v>
       </c>
-      <c r="P16" t="s">
-        <v>58</v>
-      </c>
       <c r="Q16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R16" t="s">
-        <v>58</v>
-      </c>
-      <c r="S16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1821,50 +1847,50 @@
       <c r="F17">
         <v>-1</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>-1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>58</v>
-      </c>
-      <c r="K17">
-        <v>-1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>-1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17">
+        <v>-1</v>
       </c>
       <c r="M17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N17" t="s">
         <v>37</v>
       </c>
-      <c r="N17" t="s">
-        <v>58</v>
-      </c>
       <c r="O17" t="s">
+        <v>58</v>
+      </c>
+      <c r="P17" t="s">
         <v>13</v>
       </c>
-      <c r="P17" t="s">
-        <v>58</v>
-      </c>
       <c r="Q17" t="s">
+        <v>58</v>
+      </c>
+      <c r="R17" t="s">
         <v>69</v>
       </c>
-      <c r="R17" t="s">
-        <v>58</v>
-      </c>
       <c r="S17" t="s">
         <v>58</v>
       </c>
       <c r="T17" t="s">
+        <v>58</v>
+      </c>
+      <c r="U17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1880,50 +1906,50 @@
       <c r="F18">
         <v>-1</v>
       </c>
-      <c r="G18">
-        <v>-1</v>
-      </c>
       <c r="H18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I18">
-        <v>-1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18">
-        <v>-1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>-1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18">
+        <v>-1</v>
       </c>
       <c r="M18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" t="s">
         <v>38</v>
       </c>
-      <c r="N18" t="s">
-        <v>58</v>
-      </c>
       <c r="O18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" t="s">
         <v>14</v>
       </c>
-      <c r="P18" t="s">
-        <v>58</v>
-      </c>
       <c r="Q18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R18" t="s">
-        <v>58</v>
-      </c>
-      <c r="S18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1939,50 +1965,53 @@
       <c r="F19">
         <v>-1</v>
       </c>
-      <c r="G19">
-        <v>1</v>
+      <c r="G19" t="s">
+        <v>57</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>-1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19">
-        <v>-1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>-1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19">
+        <v>-1</v>
       </c>
       <c r="M19" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" t="s">
         <v>37</v>
       </c>
-      <c r="N19" t="s">
-        <v>58</v>
-      </c>
       <c r="O19" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" t="s">
         <v>15</v>
       </c>
-      <c r="P19" t="s">
-        <v>58</v>
-      </c>
       <c r="Q19" t="s">
+        <v>58</v>
+      </c>
+      <c r="R19" t="s">
         <v>69</v>
       </c>
-      <c r="R19" t="s">
-        <v>58</v>
-      </c>
       <c r="S19" t="s">
         <v>58</v>
       </c>
       <c r="T19" t="s">
+        <v>58</v>
+      </c>
+      <c r="U19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1998,50 +2027,50 @@
       <c r="F20">
         <v>-1</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
-        <v>-1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20">
-        <v>-1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>-1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20">
+        <v>-1</v>
       </c>
       <c r="M20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
         <v>38</v>
       </c>
-      <c r="N20" t="s">
-        <v>58</v>
-      </c>
       <c r="O20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20" t="s">
         <v>16</v>
       </c>
-      <c r="P20" t="s">
-        <v>58</v>
-      </c>
       <c r="Q20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R20" t="s">
-        <v>58</v>
-      </c>
-      <c r="S20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S20" t="s">
+        <v>58</v>
+      </c>
+      <c r="T20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2057,50 +2086,53 @@
       <c r="F21">
         <v>-1</v>
       </c>
-      <c r="G21">
-        <v>1</v>
+      <c r="G21" t="s">
+        <v>57</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
-        <v>-1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21">
-        <v>-1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>-1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21">
+        <v>-1</v>
       </c>
       <c r="M21" t="s">
+        <v>57</v>
+      </c>
+      <c r="N21" t="s">
         <v>38</v>
       </c>
-      <c r="N21" t="s">
-        <v>58</v>
-      </c>
       <c r="O21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P21" t="s">
         <v>17</v>
       </c>
-      <c r="P21" t="s">
-        <v>58</v>
-      </c>
       <c r="Q21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R21" t="s">
-        <v>58</v>
-      </c>
-      <c r="S21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S21" t="s">
+        <v>58</v>
+      </c>
+      <c r="T21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2116,50 +2148,50 @@
       <c r="F22">
         <v>-1</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>-1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22">
-        <v>-1</v>
-      </c>
-      <c r="L22" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>-1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22">
+        <v>-1</v>
       </c>
       <c r="M22" t="s">
+        <v>58</v>
+      </c>
+      <c r="N22" t="s">
         <v>37</v>
       </c>
-      <c r="N22" t="s">
-        <v>58</v>
-      </c>
       <c r="O22" t="s">
+        <v>58</v>
+      </c>
+      <c r="P22" t="s">
         <v>18</v>
       </c>
-      <c r="P22" t="s">
-        <v>58</v>
-      </c>
       <c r="Q22" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" t="s">
         <v>69</v>
       </c>
-      <c r="R22" t="s">
-        <v>58</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="S22" t="s">
+        <v>58</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2175,50 +2207,53 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23">
-        <v>1</v>
+      <c r="G23" t="s">
+        <v>59</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
-        <v>-1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>-1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
         <v>59</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>37</v>
       </c>
-      <c r="N23" t="s">
-        <v>58</v>
-      </c>
       <c r="O23" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23" t="s">
         <v>19</v>
       </c>
-      <c r="P23" t="s">
-        <v>58</v>
-      </c>
       <c r="Q23" t="s">
+        <v>58</v>
+      </c>
+      <c r="R23" t="s">
         <v>59</v>
       </c>
-      <c r="R23" t="s">
-        <v>58</v>
-      </c>
-      <c r="S23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="T23" t="s">
+      <c r="S23" t="s">
+        <v>58</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2234,50 +2269,53 @@
       <c r="F24">
         <v>-1</v>
       </c>
-      <c r="G24">
-        <v>1</v>
+      <c r="G24" t="s">
+        <v>57</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>-1</v>
-      </c>
-      <c r="J24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24">
-        <v>-1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>-1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24">
+        <v>-1</v>
       </c>
       <c r="M24" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" t="s">
         <v>38</v>
       </c>
-      <c r="N24" t="s">
-        <v>58</v>
-      </c>
       <c r="O24" t="s">
+        <v>58</v>
+      </c>
+      <c r="P24" t="s">
         <v>20</v>
       </c>
-      <c r="P24" t="s">
-        <v>58</v>
-      </c>
       <c r="Q24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R24" t="s">
-        <v>58</v>
-      </c>
-      <c r="S24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S24" t="s">
+        <v>58</v>
+      </c>
+      <c r="T24" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2293,50 +2331,53 @@
       <c r="F25">
         <v>-1</v>
       </c>
-      <c r="G25">
-        <v>1</v>
+      <c r="G25" t="s">
+        <v>57</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
-        <v>-1</v>
-      </c>
-      <c r="J25" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25">
-        <v>-1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>-1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25">
+        <v>-1</v>
       </c>
       <c r="M25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" t="s">
         <v>38</v>
       </c>
-      <c r="N25" t="s">
-        <v>58</v>
-      </c>
       <c r="O25" t="s">
+        <v>58</v>
+      </c>
+      <c r="P25" t="s">
         <v>21</v>
       </c>
-      <c r="P25" t="s">
-        <v>58</v>
-      </c>
       <c r="Q25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R25" t="s">
-        <v>58</v>
-      </c>
-      <c r="S25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S25" t="s">
+        <v>58</v>
+      </c>
+      <c r="T25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2355,50 +2396,53 @@
       <c r="F26">
         <v>-1</v>
       </c>
-      <c r="G26">
-        <v>1</v>
+      <c r="G26" t="s">
+        <v>63</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26">
-        <v>-1</v>
-      </c>
-      <c r="J26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>-1</v>
+      </c>
+      <c r="K26" t="s">
         <v>63</v>
       </c>
-      <c r="K26">
-        <v>-1</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="L26">
+        <v>-1</v>
+      </c>
+      <c r="M26" t="s">
         <v>63</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>39</v>
       </c>
-      <c r="N26" t="s">
-        <v>58</v>
-      </c>
       <c r="O26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P26" t="s">
         <v>22</v>
       </c>
-      <c r="P26" t="s">
-        <v>58</v>
-      </c>
       <c r="Q26" t="s">
+        <v>58</v>
+      </c>
+      <c r="R26" t="s">
         <v>63</v>
       </c>
-      <c r="R26" t="s">
-        <v>58</v>
-      </c>
       <c r="S26" t="s">
+        <v>58</v>
+      </c>
+      <c r="T26" t="s">
         <v>63</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2414,50 +2458,53 @@
       <c r="F27">
         <v>-1</v>
       </c>
-      <c r="G27">
-        <v>1</v>
+      <c r="G27" t="s">
+        <v>57</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>-1</v>
-      </c>
-      <c r="J27" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27">
-        <v>-1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>-1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L27">
+        <v>-1</v>
       </c>
       <c r="M27" t="s">
+        <v>57</v>
+      </c>
+      <c r="N27" t="s">
         <v>42</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>51</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>23</v>
       </c>
-      <c r="P27" t="s">
-        <v>58</v>
-      </c>
       <c r="Q27" t="s">
+        <v>58</v>
+      </c>
+      <c r="R27" t="s">
         <v>70</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>51</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>92</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2473,50 +2520,53 @@
       <c r="F28">
         <v>-1</v>
       </c>
-      <c r="G28">
-        <v>1</v>
+      <c r="G28" t="s">
+        <v>57</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>-1</v>
-      </c>
-      <c r="J28" t="s">
-        <v>58</v>
-      </c>
-      <c r="K28">
-        <v>-1</v>
-      </c>
-      <c r="L28" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>-1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28">
+        <v>-1</v>
       </c>
       <c r="M28" t="s">
+        <v>57</v>
+      </c>
+      <c r="N28" t="s">
         <v>38</v>
       </c>
-      <c r="N28" t="s">
-        <v>58</v>
-      </c>
       <c r="O28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" t="s">
         <v>24</v>
       </c>
-      <c r="P28" t="s">
-        <v>58</v>
-      </c>
       <c r="Q28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R28" t="s">
-        <v>58</v>
-      </c>
-      <c r="S28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S28" t="s">
+        <v>58</v>
+      </c>
+      <c r="T28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2535,50 +2585,53 @@
       <c r="F29">
         <v>-1</v>
       </c>
-      <c r="G29">
-        <v>1</v>
+      <c r="G29" t="s">
+        <v>63</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>-1</v>
-      </c>
-      <c r="J29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>-1</v>
+      </c>
+      <c r="K29" t="s">
         <v>63</v>
       </c>
-      <c r="K29">
-        <v>-1</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="L29">
+        <v>-1</v>
+      </c>
+      <c r="M29" t="s">
         <v>63</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>39</v>
       </c>
-      <c r="N29" t="s">
-        <v>58</v>
-      </c>
       <c r="O29" t="s">
+        <v>58</v>
+      </c>
+      <c r="P29" t="s">
         <v>25</v>
       </c>
-      <c r="P29" t="s">
-        <v>58</v>
-      </c>
       <c r="Q29" t="s">
+        <v>58</v>
+      </c>
+      <c r="R29" t="s">
         <v>63</v>
       </c>
-      <c r="R29" t="s">
-        <v>58</v>
-      </c>
       <c r="S29" t="s">
+        <v>58</v>
+      </c>
+      <c r="T29" t="s">
         <v>63</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2597,50 +2650,50 @@
       <c r="F30">
         <v>-1</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>-1</v>
-      </c>
-      <c r="J30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>-1</v>
+      </c>
+      <c r="K30" t="s">
         <v>66</v>
       </c>
-      <c r="K30">
-        <v>-1</v>
-      </c>
-      <c r="L30" t="s">
-        <v>58</v>
+      <c r="L30">
+        <v>-1</v>
       </c>
       <c r="M30" t="s">
+        <v>58</v>
+      </c>
+      <c r="N30" t="s">
         <v>43</v>
       </c>
-      <c r="N30" t="s">
-        <v>58</v>
-      </c>
       <c r="O30" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" t="s">
         <v>26</v>
       </c>
-      <c r="P30" t="s">
-        <v>58</v>
-      </c>
       <c r="Q30" t="s">
+        <v>58</v>
+      </c>
+      <c r="R30" t="s">
         <v>66</v>
       </c>
-      <c r="R30" t="s">
-        <v>58</v>
-      </c>
       <c r="S30" t="s">
+        <v>58</v>
+      </c>
+      <c r="T30" t="s">
         <v>93</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2659,50 +2712,53 @@
       <c r="F31">
         <v>-1</v>
       </c>
-      <c r="G31">
-        <v>1</v>
+      <c r="G31" t="s">
+        <v>136</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
-        <v>-1</v>
-      </c>
-      <c r="J31" t="s">
-        <v>58</v>
-      </c>
-      <c r="K31">
-        <v>-1</v>
-      </c>
-      <c r="L31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>-1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>58</v>
+      </c>
+      <c r="L31">
+        <v>-1</v>
+      </c>
+      <c r="M31" t="s">
         <v>62</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>44</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>48</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>27</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>48</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>62</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>52</v>
       </c>
-      <c r="S31" s="7" t="s">
+      <c r="T31" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2718,50 +2774,53 @@
       <c r="F32">
         <v>-1</v>
       </c>
-      <c r="G32">
-        <v>1</v>
+      <c r="G32" t="s">
+        <v>57</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <v>-1</v>
-      </c>
-      <c r="J32" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32">
-        <v>-1</v>
-      </c>
-      <c r="L32" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>-1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32">
+        <v>-1</v>
       </c>
       <c r="M32" t="s">
+        <v>57</v>
+      </c>
+      <c r="N32" t="s">
         <v>42</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>51</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>28</v>
       </c>
-      <c r="P32" t="s">
-        <v>58</v>
-      </c>
       <c r="Q32" t="s">
+        <v>58</v>
+      </c>
+      <c r="R32" t="s">
         <v>70</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>51</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>92</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2777,50 +2836,53 @@
       <c r="F33">
         <v>-1</v>
       </c>
-      <c r="G33">
-        <v>1</v>
+      <c r="G33" t="s">
+        <v>57</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
-        <v>-1</v>
-      </c>
-      <c r="J33" t="s">
-        <v>58</v>
-      </c>
-      <c r="K33">
-        <v>-1</v>
-      </c>
-      <c r="L33" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>-1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L33">
+        <v>-1</v>
       </c>
       <c r="M33" t="s">
+        <v>57</v>
+      </c>
+      <c r="N33" t="s">
         <v>38</v>
       </c>
-      <c r="N33" t="s">
-        <v>58</v>
-      </c>
       <c r="O33" t="s">
+        <v>58</v>
+      </c>
+      <c r="P33" t="s">
         <v>29</v>
       </c>
-      <c r="P33" t="s">
-        <v>58</v>
-      </c>
       <c r="Q33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R33" t="s">
-        <v>58</v>
-      </c>
-      <c r="S33" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S33" t="s">
+        <v>58</v>
+      </c>
+      <c r="T33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2836,50 +2898,53 @@
       <c r="F34">
         <v>-1</v>
       </c>
-      <c r="G34">
-        <v>1</v>
+      <c r="G34" t="s">
+        <v>57</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <v>-1</v>
-      </c>
-      <c r="J34" t="s">
-        <v>58</v>
-      </c>
-      <c r="K34">
-        <v>-1</v>
-      </c>
-      <c r="L34" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>-1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>58</v>
+      </c>
+      <c r="L34">
+        <v>-1</v>
       </c>
       <c r="M34" t="s">
+        <v>57</v>
+      </c>
+      <c r="N34" t="s">
         <v>38</v>
       </c>
-      <c r="N34" t="s">
-        <v>58</v>
-      </c>
       <c r="O34" t="s">
+        <v>58</v>
+      </c>
+      <c r="P34" t="s">
         <v>30</v>
       </c>
-      <c r="P34" t="s">
-        <v>58</v>
-      </c>
       <c r="Q34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R34" t="s">
-        <v>58</v>
-      </c>
-      <c r="S34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S34" t="s">
+        <v>58</v>
+      </c>
+      <c r="T34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2895,50 +2960,53 @@
       <c r="F35">
         <v>-1</v>
       </c>
-      <c r="G35">
-        <v>1</v>
+      <c r="G35" t="s">
+        <v>57</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35">
-        <v>-1</v>
-      </c>
-      <c r="J35" t="s">
-        <v>58</v>
-      </c>
-      <c r="K35">
-        <v>-1</v>
-      </c>
-      <c r="L35" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>-1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>58</v>
+      </c>
+      <c r="L35">
+        <v>-1</v>
       </c>
       <c r="M35" t="s">
+        <v>57</v>
+      </c>
+      <c r="N35" t="s">
         <v>38</v>
       </c>
-      <c r="N35" t="s">
-        <v>58</v>
-      </c>
       <c r="O35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" t="s">
         <v>31</v>
       </c>
-      <c r="P35" t="s">
-        <v>58</v>
-      </c>
       <c r="Q35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R35" t="s">
-        <v>58</v>
-      </c>
-      <c r="S35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S35" t="s">
+        <v>58</v>
+      </c>
+      <c r="T35" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2954,50 +3022,50 @@
       <c r="F36">
         <v>-1</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>-1</v>
-      </c>
-      <c r="J36" t="s">
-        <v>58</v>
-      </c>
-      <c r="K36">
-        <v>-1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>-1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>58</v>
+      </c>
+      <c r="L36">
+        <v>-1</v>
       </c>
       <c r="M36" t="s">
+        <v>58</v>
+      </c>
+      <c r="N36" t="s">
         <v>37</v>
       </c>
-      <c r="N36" t="s">
-        <v>58</v>
-      </c>
       <c r="O36" t="s">
+        <v>58</v>
+      </c>
+      <c r="P36" t="s">
         <v>32</v>
       </c>
-      <c r="P36" t="s">
-        <v>58</v>
-      </c>
       <c r="Q36" t="s">
+        <v>58</v>
+      </c>
+      <c r="R36" t="s">
         <v>69</v>
       </c>
-      <c r="R36" t="s">
-        <v>58</v>
-      </c>
       <c r="S36" t="s">
         <v>58</v>
       </c>
       <c r="T36" t="s">
+        <v>58</v>
+      </c>
+      <c r="U36" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3013,50 +3081,50 @@
       <c r="F37">
         <v>-1</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37">
-        <v>-1</v>
-      </c>
-      <c r="J37" t="s">
-        <v>58</v>
-      </c>
-      <c r="K37">
-        <v>-1</v>
-      </c>
-      <c r="L37" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>-1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>58</v>
+      </c>
+      <c r="L37">
+        <v>-1</v>
       </c>
       <c r="M37" t="s">
+        <v>58</v>
+      </c>
+      <c r="N37" t="s">
         <v>37</v>
       </c>
-      <c r="N37" t="s">
-        <v>58</v>
-      </c>
       <c r="O37" t="s">
+        <v>58</v>
+      </c>
+      <c r="P37" t="s">
         <v>33</v>
       </c>
-      <c r="P37" t="s">
-        <v>58</v>
-      </c>
       <c r="Q37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R37" t="s">
         <v>69</v>
       </c>
-      <c r="R37" t="s">
-        <v>58</v>
-      </c>
       <c r="S37" t="s">
         <v>58</v>
       </c>
       <c r="T37" t="s">
+        <v>58</v>
+      </c>
+      <c r="U37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3075,50 +3143,53 @@
       <c r="F38">
         <v>-1</v>
       </c>
-      <c r="G38">
-        <v>1</v>
+      <c r="G38" t="s">
+        <v>68</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38">
-        <v>-1</v>
-      </c>
-      <c r="J38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>-1</v>
+      </c>
+      <c r="K38" t="s">
         <v>61</v>
       </c>
-      <c r="K38">
-        <v>-1</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="L38">
+        <v>-1</v>
+      </c>
+      <c r="M38" t="s">
         <v>68</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>40</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>50</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>34</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>49</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>68</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>49</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>95</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3137,50 +3208,50 @@
       <c r="F39">
         <v>-1</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
-        <v>-1</v>
-      </c>
-      <c r="J39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>-1</v>
+      </c>
+      <c r="K39" t="s">
         <v>66</v>
       </c>
-      <c r="K39">
-        <v>-1</v>
-      </c>
-      <c r="L39" t="s">
-        <v>58</v>
+      <c r="L39">
+        <v>-1</v>
       </c>
       <c r="M39" t="s">
+        <v>58</v>
+      </c>
+      <c r="N39" t="s">
         <v>43</v>
       </c>
-      <c r="N39" t="s">
-        <v>58</v>
-      </c>
       <c r="O39" t="s">
+        <v>58</v>
+      </c>
+      <c r="P39" t="s">
         <v>35</v>
       </c>
-      <c r="P39" t="s">
-        <v>58</v>
-      </c>
       <c r="Q39" t="s">
+        <v>58</v>
+      </c>
+      <c r="R39" t="s">
         <v>66</v>
       </c>
-      <c r="R39" t="s">
-        <v>58</v>
-      </c>
       <c r="S39" t="s">
+        <v>58</v>
+      </c>
+      <c r="T39" t="s">
         <v>93</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3196,116 +3267,119 @@
       <c r="F40">
         <v>-1</v>
       </c>
-      <c r="G40">
-        <v>1</v>
+      <c r="G40" t="s">
+        <v>57</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
-        <v>-1</v>
-      </c>
-      <c r="J40" t="s">
-        <v>58</v>
-      </c>
-      <c r="K40">
-        <v>-1</v>
-      </c>
-      <c r="L40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>-1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>58</v>
+      </c>
+      <c r="L40">
+        <v>-1</v>
+      </c>
+      <c r="M40" t="s">
         <v>60</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>42</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>51</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>36</v>
       </c>
-      <c r="P40" t="s">
-        <v>58</v>
-      </c>
       <c r="Q40" t="s">
+        <v>58</v>
+      </c>
+      <c r="R40" t="s">
         <v>70</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>51</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>92</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
       <c r="I41">
-        <v>-1</v>
-      </c>
-      <c r="J41" t="s">
-        <v>58</v>
-      </c>
-      <c r="K41">
-        <v>-1</v>
-      </c>
-      <c r="L41" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>-1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>58</v>
+      </c>
+      <c r="L41">
+        <v>-1</v>
       </c>
       <c r="M41" t="s">
+        <v>58</v>
+      </c>
+      <c r="N41" t="s">
         <v>47</v>
       </c>
-      <c r="N41" t="s">
-        <v>58</v>
-      </c>
       <c r="O41" t="s">
+        <v>58</v>
+      </c>
+      <c r="P41" t="s">
         <v>46</v>
       </c>
-      <c r="P41" t="s">
-        <v>58</v>
-      </c>
       <c r="Q41" t="s">
+        <v>58</v>
+      </c>
+      <c r="R41" t="s">
         <v>69</v>
       </c>
-      <c r="R41" t="s">
-        <v>58</v>
-      </c>
       <c r="S41" t="s">
         <v>58</v>
       </c>
       <c r="T41" t="s">
+        <v>58</v>
+      </c>
+      <c r="U41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>54</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>53</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>55</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added additional information in column headers for making them screen reader friendly
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="146">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -256,36 +256,6 @@
     <t>Tool / Screen reader</t>
   </si>
   <si>
-    <t>builtin inspector</t>
-  </si>
-  <si>
-    <t>accessibility insights</t>
-  </si>
-  <si>
-    <t>JAWS 2021</t>
-  </si>
-  <si>
-    <t>NVDA 2021</t>
-  </si>
-  <si>
-    <t>inspector</t>
-  </si>
-  <si>
-    <t>NVDA 2020</t>
-  </si>
-  <si>
-    <t>spoken by JAWS</t>
-  </si>
-  <si>
-    <t>spoken by NVDA</t>
-  </si>
-  <si>
-    <t>developer console</t>
-  </si>
-  <si>
-    <t>spoken by VoiceOver</t>
-  </si>
-  <si>
     <t>iOS</t>
   </si>
   <si>
@@ -310,9 +280,6 @@
     <t>Android</t>
   </si>
   <si>
-    <t>spoken by TalkBack</t>
-  </si>
-  <si>
     <t>abstract</t>
   </si>
   <si>
@@ -428,6 +395,66 @@
   </si>
   <si>
     <t>Sseparater</t>
+  </si>
+  <si>
+    <t>builtin inspector (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>accessibility insights (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>JAWS 2021 (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>spoken by JAWS (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>NVDA 2021 (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>spoken by NVDA (Chrome on Windows)</t>
+  </si>
+  <si>
+    <t>inspector (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>accessibility insights (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>JAWS 2021 (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>spoken by JAWS (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>NVDA 2020 (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>spoken by NVDA (Firefox on Windows)</t>
+  </si>
+  <si>
+    <t>developer console (Safari on Mac)</t>
+  </si>
+  <si>
+    <t>spoken by VoiceOver (Safari on Mac)</t>
+  </si>
+  <si>
+    <t>developer console (Chrome on Mac)</t>
+  </si>
+  <si>
+    <t>spoken by VoiceOver (Chrome on Mac)</t>
+  </si>
+  <si>
+    <t>developer console (Firefox on Mac)</t>
+  </si>
+  <si>
+    <t>spoken by VoiceOver (Firefox on Mac)</t>
+  </si>
+  <si>
+    <t>spoken by VoiceOver (Safari on iOS)</t>
+  </si>
+  <si>
+    <t>spoken by TalkBack (Chrome on Android)</t>
   </si>
 </sst>
 </file>
@@ -870,10 +897,10 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,10 +954,10 @@
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -977,64 +1004,64 @@
         <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -1093,7 +1120,7 @@
         <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -1152,10 +1179,10 @@
         <v>58</v>
       </c>
       <c r="T5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -1214,10 +1241,10 @@
         <v>58</v>
       </c>
       <c r="T6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -1276,10 +1303,10 @@
         <v>58</v>
       </c>
       <c r="T7" t="s">
+        <v>80</v>
+      </c>
+      <c r="U7" t="s">
         <v>90</v>
-      </c>
-      <c r="U7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -1296,7 +1323,7 @@
         <v>-1</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -1344,7 +1371,7 @@
         <v>63</v>
       </c>
       <c r="U8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -1403,7 +1430,7 @@
         <v>58</v>
       </c>
       <c r="T9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U9" t="s">
         <v>58</v>
@@ -1423,7 +1450,7 @@
         <v>-1</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -1471,7 +1498,7 @@
         <v>63</v>
       </c>
       <c r="U10" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -1527,10 +1554,10 @@
         <v>58</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U11" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -1589,7 +1616,7 @@
         <v>58</v>
       </c>
       <c r="U12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -1645,10 +1672,10 @@
         <v>58</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -1665,7 +1692,7 @@
         <v>-1</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -1707,10 +1734,10 @@
         <v>58</v>
       </c>
       <c r="T14" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="U14" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
@@ -1769,7 +1796,7 @@
         <v>58</v>
       </c>
       <c r="U15" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1825,10 +1852,10 @@
         <v>58</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U16" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -1887,7 +1914,7 @@
         <v>58</v>
       </c>
       <c r="U17" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
@@ -1943,7 +1970,7 @@
         <v>58</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U18" t="s">
         <v>58</v>
@@ -2008,7 +2035,7 @@
         <v>58</v>
       </c>
       <c r="U19" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -2064,10 +2091,10 @@
         <v>58</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U20" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -2126,10 +2153,10 @@
         <v>58</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U21" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
@@ -2188,7 +2215,7 @@
         <v>58</v>
       </c>
       <c r="U22" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
@@ -2309,10 +2336,10 @@
         <v>58</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U24" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -2371,10 +2398,10 @@
         <v>58</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U25" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -2391,7 +2418,7 @@
         <v>-1</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F26">
         <v>-1</v>
@@ -2439,7 +2466,7 @@
         <v>63</v>
       </c>
       <c r="U26" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
@@ -2498,10 +2525,10 @@
         <v>51</v>
       </c>
       <c r="T27" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="U27" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
@@ -2560,10 +2587,10 @@
         <v>58</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U28" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
@@ -2628,7 +2655,7 @@
         <v>63</v>
       </c>
       <c r="U29" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -2687,10 +2714,10 @@
         <v>58</v>
       </c>
       <c r="T30" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="U30" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -2707,13 +2734,13 @@
         <v>-1</v>
       </c>
       <c r="E31" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F31">
         <v>-1</v>
       </c>
       <c r="G31" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2752,10 +2779,10 @@
         <v>52</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="U31" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
@@ -2814,10 +2841,10 @@
         <v>51</v>
       </c>
       <c r="T32" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="U32" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.35">
@@ -2876,10 +2903,10 @@
         <v>58</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U33" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.35">
@@ -2938,10 +2965,10 @@
         <v>58</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U34" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.35">
@@ -3000,10 +3027,10 @@
         <v>58</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U35" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.35">
@@ -3062,7 +3089,7 @@
         <v>58</v>
       </c>
       <c r="U36" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.35">
@@ -3121,7 +3148,7 @@
         <v>58</v>
       </c>
       <c r="U37" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -3138,7 +3165,7 @@
         <v>-1</v>
       </c>
       <c r="E38" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F38">
         <v>-1</v>
@@ -3183,10 +3210,10 @@
         <v>49</v>
       </c>
       <c r="T38" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="U38" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -3245,10 +3272,10 @@
         <v>58</v>
       </c>
       <c r="T39" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="U39" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
@@ -3307,10 +3334,10 @@
         <v>51</v>
       </c>
       <c r="T40" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="U40" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
replaced 1 and 0 boolean values with the string exposed by developer inspector tool and accessibility insight tool
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="146">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -897,10 +897,10 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="S32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1068,11 +1068,11 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
       </c>
       <c r="D4">
         <v>-1</v>
@@ -1080,11 +1080,11 @@
       <c r="F4">
         <v>-1</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
       </c>
       <c r="J4">
         <v>-1</v>
@@ -1127,10 +1127,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
@@ -1142,10 +1142,10 @@
       <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
         <v>1</v>
       </c>
       <c r="J5">
@@ -1189,11 +1189,11 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
       </c>
       <c r="D6">
         <v>-1</v>
@@ -1204,11 +1204,11 @@
       <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
       </c>
       <c r="J6">
         <v>-1</v>
@@ -1251,11 +1251,11 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -1266,11 +1266,11 @@
       <c r="G7" t="s">
         <v>57</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
       </c>
       <c r="J7">
         <v>-1</v>
@@ -1313,11 +1313,11 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
       </c>
       <c r="D8">
         <v>-1</v>
@@ -1331,11 +1331,11 @@
       <c r="G8" t="s">
         <v>63</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
       </c>
       <c r="J8">
         <v>-1</v>
@@ -1378,11 +1378,11 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -1393,11 +1393,11 @@
       <c r="G9" t="s">
         <v>57</v>
       </c>
-      <c r="H9">
-        <v>-1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
       </c>
       <c r="J9">
         <v>-1</v>
@@ -1440,11 +1440,11 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -1458,11 +1458,11 @@
       <c r="G10" t="s">
         <v>63</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
       </c>
       <c r="J10">
         <v>-1</v>
@@ -1505,11 +1505,11 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -1517,11 +1517,11 @@
       <c r="F11">
         <v>-1</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
       </c>
       <c r="J11">
         <v>-1</v>
@@ -1564,11 +1564,11 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>-1</v>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1576,11 +1576,11 @@
       <c r="F12">
         <v>-1</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
       </c>
       <c r="J12">
         <v>-1</v>
@@ -1623,11 +1623,11 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -1635,11 +1635,11 @@
       <c r="F13">
         <v>-1</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
       </c>
       <c r="J13">
         <v>-1</v>
@@ -1682,11 +1682,11 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
       </c>
       <c r="D14">
         <v>-1</v>
@@ -1697,11 +1697,11 @@
       <c r="F14">
         <v>-1</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
       </c>
       <c r="J14">
         <v>-1</v>
@@ -1744,11 +1744,11 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>-1</v>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
       </c>
       <c r="D15">
         <v>-1</v>
@@ -1756,11 +1756,11 @@
       <c r="F15">
         <v>-1</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
       </c>
       <c r="J15">
         <v>-1</v>
@@ -1803,11 +1803,11 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
       </c>
       <c r="D16">
         <v>-1</v>
@@ -1815,11 +1815,11 @@
       <c r="F16">
         <v>-1</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
       </c>
       <c r="J16">
         <v>-1</v>
@@ -1862,11 +1862,11 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>-1</v>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
       </c>
       <c r="D17">
         <v>-1</v>
@@ -1874,11 +1874,11 @@
       <c r="F17">
         <v>-1</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
       </c>
       <c r="J17">
         <v>-1</v>
@@ -1921,11 +1921,11 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1933,11 +1933,11 @@
       <c r="F18">
         <v>-1</v>
       </c>
-      <c r="H18">
-        <v>-1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
       </c>
       <c r="J18">
         <v>-1</v>
@@ -1980,11 +1980,11 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>-1</v>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
       </c>
       <c r="D19">
         <v>-1</v>
@@ -1995,11 +1995,11 @@
       <c r="G19" t="s">
         <v>57</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
       </c>
       <c r="J19">
         <v>-1</v>
@@ -2042,11 +2042,11 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -2054,11 +2054,11 @@
       <c r="F20">
         <v>-1</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
       </c>
       <c r="J20">
         <v>-1</v>
@@ -2101,11 +2101,11 @@
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -2116,11 +2116,11 @@
       <c r="G21" t="s">
         <v>57</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
       </c>
       <c r="J21">
         <v>-1</v>
@@ -2163,11 +2163,11 @@
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>-1</v>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
       </c>
       <c r="D22">
         <v>-1</v>
@@ -2175,11 +2175,11 @@
       <c r="F22">
         <v>-1</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
+        <v>18</v>
       </c>
       <c r="J22">
         <v>-1</v>
@@ -2222,11 +2222,11 @@
       <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
       </c>
       <c r="D23">
         <v>-1</v>
@@ -2237,11 +2237,11 @@
       <c r="G23" t="s">
         <v>59</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
       </c>
       <c r="J23">
         <v>-1</v>
@@ -2284,11 +2284,11 @@
       <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
       <c r="D24">
         <v>-1</v>
@@ -2299,11 +2299,11 @@
       <c r="G24" t="s">
         <v>57</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
       </c>
       <c r="J24">
         <v>-1</v>
@@ -2346,11 +2346,11 @@
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
       </c>
       <c r="D25">
         <v>-1</v>
@@ -2361,11 +2361,11 @@
       <c r="G25" t="s">
         <v>57</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
       </c>
       <c r="J25">
         <v>-1</v>
@@ -2408,11 +2408,11 @@
       <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
       </c>
       <c r="D26">
         <v>-1</v>
@@ -2426,11 +2426,11 @@
       <c r="G26" t="s">
         <v>63</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
       </c>
       <c r="J26">
         <v>-1</v>
@@ -2473,11 +2473,11 @@
       <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
       </c>
       <c r="D27">
         <v>-1</v>
@@ -2488,11 +2488,11 @@
       <c r="G27" t="s">
         <v>57</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s">
+        <v>23</v>
       </c>
       <c r="J27">
         <v>-1</v>
@@ -2535,11 +2535,11 @@
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -2550,11 +2550,11 @@
       <c r="G28" t="s">
         <v>57</v>
       </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" t="s">
+        <v>24</v>
       </c>
       <c r="J28">
         <v>-1</v>
@@ -2597,11 +2597,11 @@
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
       </c>
       <c r="D29">
         <v>-1</v>
@@ -2615,11 +2615,11 @@
       <c r="G29" t="s">
         <v>63</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
       </c>
       <c r="J29">
         <v>-1</v>
@@ -2662,11 +2662,11 @@
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -2677,11 +2677,11 @@
       <c r="F30">
         <v>-1</v>
       </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
       </c>
       <c r="J30">
         <v>-1</v>
@@ -2724,11 +2724,11 @@
       <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
       </c>
       <c r="D31">
         <v>-1</v>
@@ -2742,11 +2742,11 @@
       <c r="G31" t="s">
         <v>125</v>
       </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
+      <c r="H31" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" t="s">
+        <v>27</v>
       </c>
       <c r="J31">
         <v>-1</v>
@@ -2789,11 +2789,11 @@
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
       </c>
       <c r="D32">
         <v>-1</v>
@@ -2804,11 +2804,11 @@
       <c r="G32" t="s">
         <v>57</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
+      <c r="H32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" t="s">
+        <v>28</v>
       </c>
       <c r="J32">
         <v>-1</v>
@@ -2851,11 +2851,11 @@
       <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
       </c>
       <c r="D33">
         <v>-1</v>
@@ -2866,11 +2866,11 @@
       <c r="G33" t="s">
         <v>57</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
+      <c r="H33" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" t="s">
+        <v>29</v>
       </c>
       <c r="J33">
         <v>-1</v>
@@ -2913,11 +2913,11 @@
       <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
       </c>
       <c r="D34">
         <v>-1</v>
@@ -2928,11 +2928,11 @@
       <c r="G34" t="s">
         <v>57</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
+      <c r="H34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" t="s">
+        <v>30</v>
       </c>
       <c r="J34">
         <v>-1</v>
@@ -2975,11 +2975,11 @@
       <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
       </c>
       <c r="D35">
         <v>-1</v>
@@ -2990,11 +2990,11 @@
       <c r="G35" t="s">
         <v>57</v>
       </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" t="s">
+        <v>31</v>
       </c>
       <c r="J35">
         <v>-1</v>
@@ -3037,11 +3037,11 @@
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>-1</v>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
       </c>
       <c r="D36">
         <v>-1</v>
@@ -3049,11 +3049,11 @@
       <c r="F36">
         <v>-1</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I36" t="s">
+        <v>32</v>
       </c>
       <c r="J36">
         <v>-1</v>
@@ -3096,11 +3096,11 @@
       <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>-1</v>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
       </c>
       <c r="D37">
         <v>-1</v>
@@ -3108,11 +3108,11 @@
       <c r="F37">
         <v>-1</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" t="s">
+        <v>33</v>
       </c>
       <c r="J37">
         <v>-1</v>
@@ -3155,11 +3155,11 @@
       <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>-1</v>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
       </c>
       <c r="D38">
         <v>-1</v>
@@ -3173,11 +3173,11 @@
       <c r="G38" t="s">
         <v>68</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
+      <c r="H38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
       </c>
       <c r="J38">
         <v>-1</v>
@@ -3220,11 +3220,11 @@
       <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
       </c>
       <c r="D39">
         <v>-1</v>
@@ -3235,11 +3235,11 @@
       <c r="F39">
         <v>-1</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
+      <c r="H39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" t="s">
+        <v>35</v>
       </c>
       <c r="J39">
         <v>-1</v>
@@ -3282,11 +3282,11 @@
       <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
       </c>
       <c r="D40">
         <v>-1</v>
@@ -3297,11 +3297,11 @@
       <c r="G40" t="s">
         <v>57</v>
       </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>1</v>
+      <c r="H40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" t="s">
+        <v>36</v>
       </c>
       <c r="J40">
         <v>-1</v>
@@ -3344,8 +3344,8 @@
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="I41">
-        <v>1</v>
+      <c r="I41" t="s">
+        <v>45</v>
       </c>
       <c r="J41">
         <v>-1</v>

</xml_diff>

<commit_message>
Added test results for Google Books on Android
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADDBDFB-3DE1-A949-AED1-134573FB54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="150">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -455,12 +456,24 @@
   </si>
   <si>
     <t>spoken by TalkBack (Chrome on Android)</t>
+  </si>
+  <si>
+    <t>- (on section), bibliography on div</t>
+  </si>
+  <si>
+    <t>- (on section), endnotes on div</t>
+  </si>
+  <si>
+    <t>Google Play Books</t>
+  </si>
+  <si>
+    <t>spoken by TalkBack (Google Play Books on Android)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,10 +579,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -590,9 +603,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -608,7 +622,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,7 +664,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,9 +697,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -718,6 +749,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -893,41 +941,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="S32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="T29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V41" sqref="V41"/>
+      <selection pane="bottomRight" activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.6328125" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -956,11 +1004,12 @@
       <c r="T1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="V1" s="13"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -995,11 +1044,14 @@
       <c r="T2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V2" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1063,8 +1115,11 @@
       <c r="U3" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V3" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1122,8 +1177,11 @@
       <c r="U4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1184,8 +1242,11 @@
       <c r="U5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1246,8 +1307,11 @@
       <c r="U6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1308,8 +1372,11 @@
       <c r="U7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1373,8 +1440,11 @@
       <c r="U8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1432,11 +1502,14 @@
       <c r="T9" t="s">
         <v>80</v>
       </c>
-      <c r="U9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U9" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="V9" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1500,8 +1573,11 @@
       <c r="U10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1559,8 +1635,11 @@
       <c r="U11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1618,8 +1697,11 @@
       <c r="U12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1677,8 +1759,11 @@
       <c r="U13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1739,8 +1824,11 @@
       <c r="U14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1798,8 +1886,11 @@
       <c r="U15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1857,8 +1948,11 @@
       <c r="U16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1916,8 +2010,11 @@
       <c r="U17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1972,11 +2069,14 @@
       <c r="T18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="U18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U18" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="V18" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2037,8 +2137,11 @@
       <c r="U19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2096,8 +2199,11 @@
       <c r="U20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2158,8 +2264,11 @@
       <c r="U21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2217,8 +2326,11 @@
       <c r="U22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2279,8 +2391,11 @@
       <c r="U23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2341,8 +2456,11 @@
       <c r="U24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2403,8 +2521,11 @@
       <c r="U25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2468,8 +2589,11 @@
       <c r="U26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2530,8 +2654,11 @@
       <c r="U27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2592,8 +2719,11 @@
       <c r="U28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2657,8 +2787,11 @@
       <c r="U29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2719,8 +2852,11 @@
       <c r="U30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2784,8 +2920,11 @@
       <c r="U31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2846,8 +2985,11 @@
       <c r="U32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2908,8 +3050,11 @@
       <c r="U33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2970,8 +3115,11 @@
       <c r="U34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3032,8 +3180,11 @@
       <c r="U35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3091,8 +3242,11 @@
       <c r="U36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3150,8 +3304,11 @@
       <c r="U37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3215,8 +3372,11 @@
       <c r="U38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3277,8 +3437,11 @@
       <c r="U39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3339,8 +3502,11 @@
       <c r="U40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3381,10 +3547,13 @@
         <v>58</v>
       </c>
       <c r="U41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="V41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3399,7 +3568,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="U1:V1"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="B2:G2"/>

</xml_diff>

<commit_message>
Added test on Aldiko Next on iOS
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADDBDFB-3DE1-A949-AED1-134573FB54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B975346-686C-D746-BDD8-857DEEF7908F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="151">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>spoken by TalkBack (Google Play Books on Android)</t>
+  </si>
+  <si>
+    <t>Aldiko Next</t>
   </si>
 </sst>
 </file>
@@ -571,9 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,6 +585,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,16 +601,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -942,13 +945,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="T29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="R27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U42" sqref="U42"/>
+      <selection pane="bottomRight" activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -972,86 +975,91 @@
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="23" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="4" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12"/>
+      <c r="V1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="V1" s="13"/>
-    </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W1" s="11"/>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="15" t="s">
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="5" t="s">
+      <c r="S2" s="16"/>
+      <c r="T2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1112,14 +1120,14 @@
       <c r="T3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1175,13 +1183,16 @@
         <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1240,13 +1251,16 @@
         <v>80</v>
       </c>
       <c r="U5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="V5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1305,13 +1319,16 @@
         <v>80</v>
       </c>
       <c r="U6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="V6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1370,13 +1387,16 @@
         <v>80</v>
       </c>
       <c r="U7" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7" t="s">
         <v>90</v>
       </c>
-      <c r="V7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1438,13 +1458,16 @@
         <v>63</v>
       </c>
       <c r="U8" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="V8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1502,14 +1525,17 @@
       <c r="T9" t="s">
         <v>80</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="U9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V9" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="V9" s="16" t="s">
+      <c r="W9" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1571,13 +1597,16 @@
         <v>63</v>
       </c>
       <c r="U10" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="V10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1629,17 +1658,20 @@
       <c r="S11" t="s">
         <v>58</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="T11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U11" t="s">
-        <v>93</v>
+      <c r="U11" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1695,13 +1727,16 @@
         <v>58</v>
       </c>
       <c r="U12" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="V12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1753,17 +1788,20 @@
       <c r="S13" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U13" t="s">
-        <v>95</v>
+      <c r="U13" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1822,13 +1860,16 @@
         <v>81</v>
       </c>
       <c r="U14" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="V14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1884,13 +1925,16 @@
         <v>58</v>
       </c>
       <c r="U15" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="V15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1942,17 +1986,20 @@
       <c r="S16" t="s">
         <v>58</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U16" t="s">
-        <v>98</v>
+      <c r="U16" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2008,13 +2055,16 @@
         <v>58</v>
       </c>
       <c r="U17" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="V17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2066,17 +2116,20 @@
       <c r="S18" t="s">
         <v>58</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U18" s="16" t="s">
+      <c r="U18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="V18" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="V18" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W18" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2135,13 +2188,16 @@
         <v>58</v>
       </c>
       <c r="U19" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="V19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2193,17 +2249,20 @@
       <c r="S20" t="s">
         <v>58</v>
       </c>
-      <c r="T20" s="6" t="s">
+      <c r="T20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U20" t="s">
-        <v>101</v>
+      <c r="U20" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2258,17 +2317,20 @@
       <c r="S21" t="s">
         <v>58</v>
       </c>
-      <c r="T21" s="6" t="s">
+      <c r="T21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U21" t="s">
-        <v>102</v>
+      <c r="U21" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2320,17 +2382,20 @@
       <c r="S22" t="s">
         <v>58</v>
       </c>
-      <c r="T22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U22" t="s">
-        <v>103</v>
+      <c r="T22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="V22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2385,17 +2450,20 @@
       <c r="S23" t="s">
         <v>58</v>
       </c>
-      <c r="T23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U23" t="s">
-        <v>59</v>
+      <c r="T23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="V23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2450,17 +2518,20 @@
       <c r="S24" t="s">
         <v>58</v>
       </c>
-      <c r="T24" s="6" t="s">
+      <c r="T24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U24" t="s">
-        <v>104</v>
+      <c r="U24" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2515,17 +2586,20 @@
       <c r="S25" t="s">
         <v>58</v>
       </c>
-      <c r="T25" s="6" t="s">
+      <c r="T25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U25" t="s">
-        <v>105</v>
+      <c r="U25" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2587,13 +2661,16 @@
         <v>63</v>
       </c>
       <c r="U26" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="V26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2652,13 +2729,16 @@
         <v>82</v>
       </c>
       <c r="U27" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="V27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2713,17 +2793,20 @@
       <c r="S28" t="s">
         <v>58</v>
       </c>
-      <c r="T28" s="6" t="s">
+      <c r="T28" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U28" t="s">
-        <v>108</v>
+      <c r="U28" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2785,13 +2868,16 @@
         <v>63</v>
       </c>
       <c r="U29" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="V29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2850,13 +2936,16 @@
         <v>83</v>
       </c>
       <c r="U30" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="V30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2914,17 +3003,20 @@
       <c r="S31" t="s">
         <v>52</v>
       </c>
-      <c r="T31" s="7" t="s">
+      <c r="T31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="U31" t="s">
-        <v>111</v>
+      <c r="U31" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="V31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2983,13 +3075,16 @@
         <v>82</v>
       </c>
       <c r="U32" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="V32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3044,17 +3139,20 @@
       <c r="S33" t="s">
         <v>58</v>
       </c>
-      <c r="T33" s="6" t="s">
+      <c r="T33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U33" t="s">
-        <v>113</v>
+      <c r="U33" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3109,17 +3207,20 @@
       <c r="S34" t="s">
         <v>58</v>
       </c>
-      <c r="T34" s="6" t="s">
+      <c r="T34" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U34" t="s">
-        <v>114</v>
+      <c r="U34" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3174,17 +3275,20 @@
       <c r="S35" t="s">
         <v>58</v>
       </c>
-      <c r="T35" s="6" t="s">
+      <c r="T35" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="U35" t="s">
-        <v>115</v>
+      <c r="U35" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="V35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3240,13 +3344,16 @@
         <v>58</v>
       </c>
       <c r="U36" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="V36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3302,13 +3409,16 @@
         <v>58</v>
       </c>
       <c r="U37" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="V37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3370,13 +3480,16 @@
         <v>85</v>
       </c>
       <c r="U38" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="V38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3435,13 +3548,16 @@
         <v>83</v>
       </c>
       <c r="U39" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="V39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3500,13 +3616,16 @@
         <v>82</v>
       </c>
       <c r="U40" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="V40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3552,8 +3671,11 @@
       <c r="V41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3568,8 +3690,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="U1:V1"/>
+  <mergeCells count="9">
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="B2:G2"/>
@@ -3577,6 +3699,7 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test results of Thorium 1.71 windows with JAWS 2021
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B975346-686C-D746-BDD8-857DEEF7908F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="153">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -471,12 +470,18 @@
   </si>
   <si>
     <t>Aldiko Next</t>
+  </si>
+  <si>
+    <t>Thorium RS V1.7.1</t>
+  </si>
+  <si>
+    <t>JAWS 2021 / Thorium 1.71 on Windows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -565,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -589,10 +594,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -607,9 +612,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -625,7 +636,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -667,7 +678,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,26 +711,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -752,23 +746,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -944,77 +921,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="R27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U32" sqref="U32"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" customWidth="1"/>
-    <col min="22" max="23" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" customWidth="1"/>
+    <col min="23" max="24" width="32.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="13"/>
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="13"/>
+      <c r="U1" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="12"/>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="17"/>
+      <c r="W1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="W1" s="11"/>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X1" s="12"/>
+    </row>
+    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -1035,31 +1014,34 @@
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
       <c r="N2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="16"/>
+      <c r="U2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1100,34 +1082,37 @@
         <v>137</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1162,23 +1147,23 @@
         <v>58</v>
       </c>
       <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="O4" t="s">
-        <v>58</v>
-      </c>
       <c r="P4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" t="s">
-        <v>58</v>
-      </c>
       <c r="R4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" t="s">
         <v>69</v>
       </c>
-      <c r="S4" t="s">
-        <v>58</v>
-      </c>
       <c r="T4" t="s">
         <v>58</v>
       </c>
@@ -1186,13 +1171,16 @@
         <v>58</v>
       </c>
       <c r="V4" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="W4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1230,37 +1218,40 @@
         <v>57</v>
       </c>
       <c r="N5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" t="s">
         <v>38</v>
       </c>
-      <c r="O5" t="s">
-        <v>58</v>
-      </c>
       <c r="P5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" t="s">
-        <v>58</v>
-      </c>
       <c r="R5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U5" t="s">
         <v>80</v>
       </c>
       <c r="V5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="W5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1297,38 +1288,42 @@
       <c r="M6" t="s">
         <v>57</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="e">
+        <f>-N7</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O6" t="s">
         <v>38</v>
       </c>
-      <c r="O6" t="s">
-        <v>58</v>
-      </c>
       <c r="P6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" t="s">
-        <v>58</v>
-      </c>
       <c r="R6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T6" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U6" t="s">
         <v>80</v>
       </c>
       <c r="V6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1366,37 +1361,40 @@
         <v>57</v>
       </c>
       <c r="N7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" t="s">
         <v>38</v>
       </c>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
       <c r="P7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" t="s">
-        <v>58</v>
-      </c>
       <c r="R7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T7" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U7" t="s">
         <v>80</v>
       </c>
       <c r="V7" t="s">
+        <v>80</v>
+      </c>
+      <c r="W7" t="s">
         <v>90</v>
       </c>
-      <c r="W7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1437,37 +1435,40 @@
         <v>63</v>
       </c>
       <c r="N8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s">
         <v>39</v>
       </c>
-      <c r="O8" t="s">
-        <v>58</v>
-      </c>
       <c r="P8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" t="s">
-        <v>58</v>
-      </c>
       <c r="R8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" t="s">
         <v>63</v>
       </c>
-      <c r="S8" t="s">
-        <v>58</v>
-      </c>
       <c r="T8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U8" t="s">
         <v>63</v>
       </c>
       <c r="V8" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="W8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1505,37 +1506,40 @@
         <v>57</v>
       </c>
       <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="O9" t="s">
-        <v>58</v>
-      </c>
       <c r="P9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" t="s">
         <v>5</v>
       </c>
-      <c r="Q9" t="s">
-        <v>58</v>
-      </c>
       <c r="R9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T9" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U9" t="s">
         <v>80</v>
       </c>
-      <c r="V9" s="10" t="s">
-        <v>146</v>
+      <c r="V9" t="s">
+        <v>80</v>
       </c>
       <c r="W9" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X9" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1576,37 +1580,40 @@
         <v>63</v>
       </c>
       <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" t="s">
         <v>39</v>
       </c>
-      <c r="O10" t="s">
-        <v>58</v>
-      </c>
       <c r="P10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" t="s">
-        <v>58</v>
-      </c>
       <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
         <v>63</v>
       </c>
-      <c r="S10" t="s">
-        <v>58</v>
-      </c>
       <c r="T10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U10" t="s">
         <v>63</v>
       </c>
       <c r="V10" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="W10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1641,37 +1648,40 @@
         <v>57</v>
       </c>
       <c r="N11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" t="s">
         <v>38</v>
       </c>
-      <c r="O11" t="s">
-        <v>58</v>
-      </c>
       <c r="P11" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q11" t="s">
         <v>7</v>
       </c>
-      <c r="Q11" t="s">
-        <v>58</v>
-      </c>
       <c r="R11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S11" t="s">
-        <v>58</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T11" t="s">
+        <v>58</v>
       </c>
       <c r="U11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V11" t="s">
-        <v>93</v>
+      <c r="V11" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1706,23 +1716,23 @@
         <v>58</v>
       </c>
       <c r="N12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" t="s">
         <v>37</v>
       </c>
-      <c r="O12" t="s">
-        <v>58</v>
-      </c>
       <c r="P12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" t="s">
-        <v>58</v>
-      </c>
       <c r="R12" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" t="s">
         <v>69</v>
       </c>
-      <c r="S12" t="s">
-        <v>58</v>
-      </c>
       <c r="T12" t="s">
         <v>58</v>
       </c>
@@ -1730,13 +1740,16 @@
         <v>58</v>
       </c>
       <c r="V12" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="W12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1771,37 +1784,40 @@
         <v>57</v>
       </c>
       <c r="N13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" t="s">
         <v>38</v>
       </c>
-      <c r="O13" t="s">
-        <v>58</v>
-      </c>
       <c r="P13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" t="s">
         <v>9</v>
       </c>
-      <c r="Q13" t="s">
-        <v>58</v>
-      </c>
       <c r="R13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S13" t="s">
-        <v>58</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T13" t="s">
+        <v>58</v>
       </c>
       <c r="U13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V13" t="s">
-        <v>95</v>
+      <c r="V13" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1839,37 +1855,40 @@
         <v>65</v>
       </c>
       <c r="N14" t="s">
+        <v>65</v>
+      </c>
+      <c r="O14" t="s">
         <v>41</v>
       </c>
-      <c r="O14" t="s">
-        <v>58</v>
-      </c>
       <c r="P14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" t="s">
         <v>10</v>
       </c>
-      <c r="Q14" t="s">
-        <v>58</v>
-      </c>
       <c r="R14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S14" t="s">
         <v>65</v>
       </c>
-      <c r="S14" t="s">
-        <v>58</v>
-      </c>
       <c r="T14" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="U14" t="s">
         <v>81</v>
       </c>
       <c r="V14" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="W14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1904,23 +1923,23 @@
         <v>58</v>
       </c>
       <c r="N15" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" t="s">
         <v>37</v>
       </c>
-      <c r="O15" t="s">
-        <v>58</v>
-      </c>
       <c r="P15" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" t="s">
         <v>11</v>
       </c>
-      <c r="Q15" t="s">
-        <v>58</v>
-      </c>
       <c r="R15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" t="s">
         <v>69</v>
       </c>
-      <c r="S15" t="s">
-        <v>58</v>
-      </c>
       <c r="T15" t="s">
         <v>58</v>
       </c>
@@ -1928,13 +1947,16 @@
         <v>58</v>
       </c>
       <c r="V15" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="W15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1969,37 +1991,40 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
         <v>38</v>
       </c>
-      <c r="O16" t="s">
-        <v>58</v>
-      </c>
       <c r="P16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q16" t="s">
         <v>12</v>
       </c>
-      <c r="Q16" t="s">
-        <v>58</v>
-      </c>
       <c r="R16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T16" t="s">
+        <v>58</v>
       </c>
       <c r="U16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V16" t="s">
-        <v>98</v>
+      <c r="V16" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2034,23 +2059,23 @@
         <v>58</v>
       </c>
       <c r="N17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" t="s">
         <v>37</v>
       </c>
-      <c r="O17" t="s">
-        <v>58</v>
-      </c>
       <c r="P17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q17" t="s">
         <v>13</v>
       </c>
-      <c r="Q17" t="s">
-        <v>58</v>
-      </c>
       <c r="R17" t="s">
+        <v>58</v>
+      </c>
+      <c r="S17" t="s">
         <v>69</v>
       </c>
-      <c r="S17" t="s">
-        <v>58</v>
-      </c>
       <c r="T17" t="s">
         <v>58</v>
       </c>
@@ -2058,13 +2083,16 @@
         <v>58</v>
       </c>
       <c r="V17" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="W17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2099,37 +2127,40 @@
         <v>57</v>
       </c>
       <c r="N18" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" t="s">
         <v>38</v>
       </c>
-      <c r="O18" t="s">
-        <v>58</v>
-      </c>
       <c r="P18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" t="s">
         <v>14</v>
       </c>
-      <c r="Q18" t="s">
-        <v>58</v>
-      </c>
       <c r="R18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S18" t="s">
-        <v>58</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T18" t="s">
+        <v>58</v>
       </c>
       <c r="U18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V18" s="10" t="s">
+      <c r="V18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="W18" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="W18" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2167,23 +2198,23 @@
         <v>58</v>
       </c>
       <c r="N19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O19" t="s">
         <v>37</v>
       </c>
-      <c r="O19" t="s">
-        <v>58</v>
-      </c>
       <c r="P19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q19" t="s">
         <v>15</v>
       </c>
-      <c r="Q19" t="s">
-        <v>58</v>
-      </c>
       <c r="R19" t="s">
+        <v>58</v>
+      </c>
+      <c r="S19" t="s">
         <v>69</v>
       </c>
-      <c r="S19" t="s">
-        <v>58</v>
-      </c>
       <c r="T19" t="s">
         <v>58</v>
       </c>
@@ -2191,13 +2222,16 @@
         <v>58</v>
       </c>
       <c r="V19" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="W19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2232,37 +2266,40 @@
         <v>57</v>
       </c>
       <c r="N20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O20" t="s">
         <v>38</v>
       </c>
-      <c r="O20" t="s">
-        <v>58</v>
-      </c>
       <c r="P20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q20" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" t="s">
-        <v>58</v>
-      </c>
       <c r="R20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S20" t="s">
-        <v>58</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T20" t="s">
+        <v>58</v>
       </c>
       <c r="U20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V20" t="s">
-        <v>101</v>
+      <c r="V20" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2300,37 +2337,40 @@
         <v>57</v>
       </c>
       <c r="N21" t="s">
+        <v>58</v>
+      </c>
+      <c r="O21" t="s">
         <v>38</v>
       </c>
-      <c r="O21" t="s">
-        <v>58</v>
-      </c>
       <c r="P21" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q21" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" t="s">
-        <v>58</v>
-      </c>
       <c r="R21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S21" t="s">
-        <v>58</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T21" t="s">
+        <v>58</v>
       </c>
       <c r="U21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V21" t="s">
-        <v>102</v>
+      <c r="V21" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2365,37 +2405,40 @@
         <v>58</v>
       </c>
       <c r="N22" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" t="s">
         <v>37</v>
       </c>
-      <c r="O22" t="s">
-        <v>58</v>
-      </c>
       <c r="P22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q22" t="s">
         <v>18</v>
       </c>
-      <c r="Q22" t="s">
-        <v>58</v>
-      </c>
       <c r="R22" t="s">
+        <v>58</v>
+      </c>
+      <c r="S22" t="s">
         <v>69</v>
       </c>
-      <c r="S22" t="s">
-        <v>58</v>
-      </c>
-      <c r="T22" s="5" t="s">
+      <c r="T22" t="s">
         <v>58</v>
       </c>
       <c r="U22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V22" t="s">
-        <v>103</v>
+      <c r="V22" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="W22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2433,37 +2476,40 @@
         <v>59</v>
       </c>
       <c r="N23" t="s">
+        <v>58</v>
+      </c>
+      <c r="O23" t="s">
         <v>37</v>
       </c>
-      <c r="O23" t="s">
-        <v>58</v>
-      </c>
       <c r="P23" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q23" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" t="s">
-        <v>58</v>
-      </c>
       <c r="R23" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" t="s">
         <v>59</v>
       </c>
-      <c r="S23" t="s">
-        <v>58</v>
-      </c>
-      <c r="T23" s="5" t="s">
+      <c r="T23" t="s">
         <v>58</v>
       </c>
       <c r="U23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V23" t="s">
-        <v>59</v>
+      <c r="V23" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="W23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2501,37 +2547,40 @@
         <v>57</v>
       </c>
       <c r="N24" t="s">
+        <v>58</v>
+      </c>
+      <c r="O24" t="s">
         <v>38</v>
       </c>
-      <c r="O24" t="s">
-        <v>58</v>
-      </c>
       <c r="P24" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q24" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" t="s">
-        <v>58</v>
-      </c>
       <c r="R24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S24" t="s">
-        <v>58</v>
-      </c>
-      <c r="T24" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T24" t="s">
+        <v>58</v>
       </c>
       <c r="U24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V24" t="s">
-        <v>104</v>
+      <c r="V24" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2569,37 +2618,40 @@
         <v>57</v>
       </c>
       <c r="N25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O25" t="s">
         <v>38</v>
       </c>
-      <c r="O25" t="s">
-        <v>58</v>
-      </c>
       <c r="P25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q25" t="s">
         <v>21</v>
       </c>
-      <c r="Q25" t="s">
-        <v>58</v>
-      </c>
       <c r="R25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S25" t="s">
-        <v>58</v>
-      </c>
-      <c r="T25" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T25" t="s">
+        <v>58</v>
       </c>
       <c r="U25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V25" t="s">
-        <v>105</v>
+      <c r="V25" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2640,37 +2692,40 @@
         <v>63</v>
       </c>
       <c r="N26" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" t="s">
         <v>39</v>
       </c>
-      <c r="O26" t="s">
-        <v>58</v>
-      </c>
       <c r="P26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" t="s">
         <v>22</v>
       </c>
-      <c r="Q26" t="s">
-        <v>58</v>
-      </c>
       <c r="R26" t="s">
+        <v>58</v>
+      </c>
+      <c r="S26" t="s">
         <v>63</v>
       </c>
-      <c r="S26" t="s">
-        <v>58</v>
-      </c>
       <c r="T26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U26" t="s">
         <v>63</v>
       </c>
       <c r="V26" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="W26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2708,37 +2763,40 @@
         <v>57</v>
       </c>
       <c r="N27" t="s">
+        <v>58</v>
+      </c>
+      <c r="O27" t="s">
         <v>42</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>51</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>23</v>
       </c>
-      <c r="Q27" t="s">
-        <v>58</v>
-      </c>
       <c r="R27" t="s">
+        <v>58</v>
+      </c>
+      <c r="S27" t="s">
         <v>70</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>51</v>
-      </c>
-      <c r="T27" t="s">
-        <v>82</v>
       </c>
       <c r="U27" t="s">
         <v>82</v>
       </c>
       <c r="V27" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="W27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2776,37 +2834,40 @@
         <v>57</v>
       </c>
       <c r="N28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O28" t="s">
         <v>38</v>
       </c>
-      <c r="O28" t="s">
-        <v>58</v>
-      </c>
       <c r="P28" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q28" t="s">
         <v>24</v>
       </c>
-      <c r="Q28" t="s">
-        <v>58</v>
-      </c>
       <c r="R28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S28" t="s">
-        <v>58</v>
-      </c>
-      <c r="T28" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T28" t="s">
+        <v>58</v>
       </c>
       <c r="U28" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V28" t="s">
-        <v>108</v>
+      <c r="V28" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2847,37 +2908,40 @@
         <v>63</v>
       </c>
       <c r="N29" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" t="s">
         <v>39</v>
       </c>
-      <c r="O29" t="s">
-        <v>58</v>
-      </c>
       <c r="P29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q29" t="s">
         <v>25</v>
       </c>
-      <c r="Q29" t="s">
-        <v>58</v>
-      </c>
       <c r="R29" t="s">
+        <v>58</v>
+      </c>
+      <c r="S29" t="s">
         <v>63</v>
       </c>
-      <c r="S29" t="s">
-        <v>58</v>
-      </c>
       <c r="T29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U29" t="s">
         <v>63</v>
       </c>
       <c r="V29" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="W29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2915,37 +2979,40 @@
         <v>58</v>
       </c>
       <c r="N30" t="s">
+        <v>66</v>
+      </c>
+      <c r="O30" t="s">
         <v>43</v>
       </c>
-      <c r="O30" t="s">
-        <v>58</v>
-      </c>
       <c r="P30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q30" t="s">
         <v>26</v>
       </c>
-      <c r="Q30" t="s">
-        <v>58</v>
-      </c>
       <c r="R30" t="s">
+        <v>58</v>
+      </c>
+      <c r="S30" t="s">
         <v>66</v>
       </c>
-      <c r="S30" t="s">
-        <v>58</v>
-      </c>
       <c r="T30" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="U30" t="s">
         <v>83</v>
       </c>
       <c r="V30" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="W30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2986,37 +3053,40 @@
         <v>62</v>
       </c>
       <c r="N31" t="s">
+        <v>62</v>
+      </c>
+      <c r="O31" t="s">
         <v>44</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>48</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>27</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>48</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>62</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>52</v>
-      </c>
-      <c r="T31" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="U31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="V31" t="s">
-        <v>111</v>
+      <c r="V31" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="W31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3054,37 +3124,40 @@
         <v>57</v>
       </c>
       <c r="N32" t="s">
+        <v>58</v>
+      </c>
+      <c r="O32" t="s">
         <v>42</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>51</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>28</v>
       </c>
-      <c r="Q32" t="s">
-        <v>58</v>
-      </c>
       <c r="R32" t="s">
+        <v>58</v>
+      </c>
+      <c r="S32" t="s">
         <v>70</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>51</v>
-      </c>
-      <c r="T32" t="s">
-        <v>82</v>
       </c>
       <c r="U32" t="s">
         <v>82</v>
       </c>
       <c r="V32" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="W32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3122,37 +3195,40 @@
         <v>57</v>
       </c>
       <c r="N33" t="s">
+        <v>58</v>
+      </c>
+      <c r="O33" t="s">
         <v>38</v>
       </c>
-      <c r="O33" t="s">
-        <v>58</v>
-      </c>
       <c r="P33" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q33" t="s">
         <v>29</v>
       </c>
-      <c r="Q33" t="s">
-        <v>58</v>
-      </c>
       <c r="R33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S33" t="s">
-        <v>58</v>
-      </c>
-      <c r="T33" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T33" t="s">
+        <v>58</v>
       </c>
       <c r="U33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V33" t="s">
-        <v>113</v>
+      <c r="V33" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3190,37 +3266,40 @@
         <v>57</v>
       </c>
       <c r="N34" t="s">
+        <v>58</v>
+      </c>
+      <c r="O34" t="s">
         <v>38</v>
       </c>
-      <c r="O34" t="s">
-        <v>58</v>
-      </c>
       <c r="P34" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q34" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" t="s">
-        <v>58</v>
-      </c>
       <c r="R34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S34" t="s">
-        <v>58</v>
-      </c>
-      <c r="T34" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T34" t="s">
+        <v>58</v>
       </c>
       <c r="U34" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V34" t="s">
-        <v>114</v>
+      <c r="V34" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3258,37 +3337,40 @@
         <v>57</v>
       </c>
       <c r="N35" t="s">
+        <v>58</v>
+      </c>
+      <c r="O35" t="s">
         <v>38</v>
       </c>
-      <c r="O35" t="s">
-        <v>58</v>
-      </c>
       <c r="P35" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q35" t="s">
         <v>31</v>
       </c>
-      <c r="Q35" t="s">
-        <v>58</v>
-      </c>
       <c r="R35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S35" t="s">
-        <v>58</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="T35" t="s">
+        <v>58</v>
       </c>
       <c r="U35" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V35" t="s">
-        <v>115</v>
+      <c r="V35" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="W35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3323,23 +3405,23 @@
         <v>58</v>
       </c>
       <c r="N36" t="s">
+        <v>58</v>
+      </c>
+      <c r="O36" t="s">
         <v>37</v>
       </c>
-      <c r="O36" t="s">
-        <v>58</v>
-      </c>
       <c r="P36" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q36" t="s">
         <v>32</v>
       </c>
-      <c r="Q36" t="s">
-        <v>58</v>
-      </c>
       <c r="R36" t="s">
+        <v>58</v>
+      </c>
+      <c r="S36" t="s">
         <v>69</v>
       </c>
-      <c r="S36" t="s">
-        <v>58</v>
-      </c>
       <c r="T36" t="s">
         <v>58</v>
       </c>
@@ -3347,13 +3429,16 @@
         <v>58</v>
       </c>
       <c r="V36" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="W36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3388,23 +3473,23 @@
         <v>58</v>
       </c>
       <c r="N37" t="s">
+        <v>58</v>
+      </c>
+      <c r="O37" t="s">
         <v>37</v>
       </c>
-      <c r="O37" t="s">
-        <v>58</v>
-      </c>
       <c r="P37" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q37" t="s">
         <v>33</v>
       </c>
-      <c r="Q37" t="s">
-        <v>58</v>
-      </c>
       <c r="R37" t="s">
+        <v>58</v>
+      </c>
+      <c r="S37" t="s">
         <v>69</v>
       </c>
-      <c r="S37" t="s">
-        <v>58</v>
-      </c>
       <c r="T37" t="s">
         <v>58</v>
       </c>
@@ -3412,13 +3497,16 @@
         <v>58</v>
       </c>
       <c r="V37" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="W37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3459,37 +3547,40 @@
         <v>68</v>
       </c>
       <c r="N38" t="s">
+        <v>68</v>
+      </c>
+      <c r="O38" t="s">
         <v>40</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>50</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>34</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>49</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>68</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>49</v>
-      </c>
-      <c r="T38" t="s">
-        <v>85</v>
       </c>
       <c r="U38" t="s">
         <v>85</v>
       </c>
       <c r="V38" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="W38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3527,37 +3618,40 @@
         <v>58</v>
       </c>
       <c r="N39" t="s">
+        <v>66</v>
+      </c>
+      <c r="O39" t="s">
         <v>43</v>
       </c>
-      <c r="O39" t="s">
-        <v>58</v>
-      </c>
       <c r="P39" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q39" t="s">
         <v>35</v>
       </c>
-      <c r="Q39" t="s">
-        <v>58</v>
-      </c>
       <c r="R39" t="s">
+        <v>58</v>
+      </c>
+      <c r="S39" t="s">
         <v>66</v>
       </c>
-      <c r="S39" t="s">
-        <v>58</v>
-      </c>
       <c r="T39" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="U39" t="s">
         <v>83</v>
       </c>
       <c r="V39" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="W39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3595,37 +3689,40 @@
         <v>60</v>
       </c>
       <c r="N40" t="s">
+        <v>58</v>
+      </c>
+      <c r="O40" t="s">
         <v>42</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>51</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>36</v>
       </c>
-      <c r="Q40" t="s">
-        <v>58</v>
-      </c>
       <c r="R40" t="s">
+        <v>58</v>
+      </c>
+      <c r="S40" t="s">
         <v>70</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>51</v>
-      </c>
-      <c r="T40" t="s">
-        <v>82</v>
       </c>
       <c r="U40" t="s">
         <v>82</v>
       </c>
       <c r="V40" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="W40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3645,23 +3742,23 @@
         <v>58</v>
       </c>
       <c r="N41" t="s">
+        <v>58</v>
+      </c>
+      <c r="O41" t="s">
         <v>47</v>
       </c>
-      <c r="O41" t="s">
-        <v>58</v>
-      </c>
       <c r="P41" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q41" t="s">
         <v>46</v>
       </c>
-      <c r="Q41" t="s">
-        <v>58</v>
-      </c>
       <c r="R41" t="s">
+        <v>58</v>
+      </c>
+      <c r="S41" t="s">
         <v>69</v>
       </c>
-      <c r="S41" t="s">
-        <v>58</v>
-      </c>
       <c r="T41" t="s">
         <v>58</v>
       </c>
@@ -3674,8 +3771,11 @@
       <c r="W41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3691,15 +3791,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O1:T1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="B1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test results of Aldiko on Android with Talkback
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F36FAA0-BEE5-A547-AE20-3FB2ABCD7EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,23 @@
   <definedNames>
     <definedName name="Title_8e133929154a42a88c65db5298a3d721" localSheetId="0">results!$A$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="155">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -476,12 +488,18 @@
   </si>
   <si>
     <t>JAWS 2021 / Thorium 1.71 on Windows</t>
+  </si>
+  <si>
+    <t>Aldiko</t>
+  </si>
+  <si>
+    <t>spoken by TalkBack (Aldiko on Android)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -570,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -597,6 +615,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,7 +641,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -636,7 +657,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -678,7 +699,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -711,9 +732,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -746,6 +784,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -921,113 +976,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="T14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.6328125" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
-    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
-    <col min="23" max="24" width="32.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.5" customWidth="1"/>
+    <col min="24" max="24" width="24.6640625" customWidth="1"/>
+    <col min="25" max="25" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="13" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="17" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="17"/>
-      <c r="W1" s="12" t="s">
+      <c r="V1" s="18"/>
+      <c r="W1" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="X1" s="12"/>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
       <c r="N2" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="15" t="s">
+      <c r="P2" s="13"/>
+      <c r="Q2" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="16" t="s">
+      <c r="R2" s="16"/>
+      <c r="S2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="16"/>
+      <c r="T2" s="17"/>
       <c r="U2" s="4" t="s">
         <v>77</v>
       </c>
@@ -1040,8 +1098,11 @@
       <c r="X2" s="8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y2" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1111,8 +1172,11 @@
       <c r="X3" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y3" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1179,8 +1243,11 @@
       <c r="X4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1250,8 +1317,11 @@
       <c r="X5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1322,8 +1392,11 @@
       <c r="X6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1393,8 +1466,11 @@
       <c r="X7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1467,8 +1543,11 @@
       <c r="X8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1538,8 +1617,11 @@
       <c r="X9" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y9" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1612,8 +1694,11 @@
       <c r="X10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1680,8 +1765,11 @@
       <c r="X11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1748,8 +1836,11 @@
       <c r="X12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1816,8 +1907,11 @@
       <c r="X13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1887,8 +1981,11 @@
       <c r="X14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1955,8 +2052,11 @@
       <c r="X15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2023,8 +2123,11 @@
       <c r="X16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2091,8 +2194,11 @@
       <c r="X17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2159,8 +2265,11 @@
       <c r="X18" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y18" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2230,8 +2339,11 @@
       <c r="X19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2298,8 +2410,11 @@
       <c r="X20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2369,8 +2484,11 @@
       <c r="X21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2437,8 +2555,11 @@
       <c r="X22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2508,8 +2629,11 @@
       <c r="X23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2579,8 +2703,11 @@
       <c r="X24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2650,8 +2777,11 @@
       <c r="X25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2724,8 +2854,11 @@
       <c r="X26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2795,8 +2928,11 @@
       <c r="X27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2866,8 +3002,11 @@
       <c r="X28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2940,8 +3079,11 @@
       <c r="X29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3011,8 +3153,11 @@
       <c r="X30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3085,8 +3230,11 @@
       <c r="X31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3156,8 +3304,11 @@
       <c r="X32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3227,8 +3378,11 @@
       <c r="X33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3298,8 +3452,11 @@
       <c r="X34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3369,8 +3526,11 @@
       <c r="X35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3437,8 +3597,11 @@
       <c r="X36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3505,8 +3668,11 @@
       <c r="X37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3579,8 +3745,11 @@
       <c r="X38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3650,8 +3819,11 @@
       <c r="X39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3721,8 +3893,11 @@
       <c r="X40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3774,8 +3949,11 @@
       <c r="X41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3791,7 +3969,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="W1:X1"/>
     <mergeCell ref="O1:T1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
@@ -3800,6 +3977,7 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="B1:N1"/>
+    <mergeCell ref="W1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
I added a column for NVDA and Thorium 1.7.1 for Windows. I did not put results in for Jaws, because it did not do anything with the roles.
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F36FAA0-BEE5-A547-AE20-3FB2ABCD7EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232B2352-7152-4DC5-9110-FAC324EF4E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="156">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>spoken by TalkBack (Aldiko on Android)</t>
+  </si>
+  <si>
+    <t>NVDA 2021-1 Thorium 1.7.1 on Windows</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -618,6 +621,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,15 +645,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -657,7 +663,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -977,132 +983,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y42"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="T14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y32" sqref="Y32"/>
+      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" customWidth="1"/>
-    <col min="23" max="23" width="25.5" customWidth="1"/>
-    <col min="24" max="24" width="24.6640625" customWidth="1"/>
-    <col min="25" max="25" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.453125" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="24" max="24" width="25.453125" customWidth="1"/>
+    <col min="25" max="25" width="24.6328125" customWidth="1"/>
+    <col min="26" max="26" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="14" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="18" t="s">
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="18"/>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="14"/>
+      <c r="X1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-    </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="11" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="19"/>
+      <c r="T2" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="17"/>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="20"/>
+      <c r="V2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Z2" s="12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -1143,40 +1151,43 @@
         <v>137</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1214,23 +1225,23 @@
         <v>58</v>
       </c>
       <c r="O4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" t="s">
         <v>37</v>
       </c>
-      <c r="P4" t="s">
-        <v>58</v>
-      </c>
       <c r="Q4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" t="s">
         <v>0</v>
       </c>
-      <c r="R4" t="s">
-        <v>58</v>
-      </c>
       <c r="S4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" t="s">
         <v>69</v>
       </c>
-      <c r="T4" t="s">
-        <v>58</v>
-      </c>
       <c r="U4" t="s">
         <v>58</v>
       </c>
@@ -1238,7 +1249,7 @@
         <v>58</v>
       </c>
       <c r="W4" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="X4" t="s">
         <v>87</v>
@@ -1246,8 +1257,11 @@
       <c r="Y4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1285,34 +1299,34 @@
         <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O5" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
-        <v>58</v>
-      </c>
       <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" t="s">
         <v>1</v>
       </c>
-      <c r="R5" t="s">
-        <v>58</v>
-      </c>
       <c r="S5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="V5" t="s">
         <v>80</v>
       </c>
       <c r="W5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="X5" t="s">
         <v>88</v>
@@ -1320,8 +1334,11 @@
       <c r="Y5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1358,36 +1375,36 @@
       <c r="M6" t="s">
         <v>57</v>
       </c>
-      <c r="N6" t="e">
-        <f>-N7</f>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" t="e">
+        <f>-O7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>38</v>
       </c>
-      <c r="P6" t="s">
-        <v>58</v>
-      </c>
       <c r="Q6" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" t="s">
         <v>2</v>
       </c>
-      <c r="R6" t="s">
-        <v>58</v>
-      </c>
       <c r="S6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U6" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="V6" t="s">
         <v>80</v>
       </c>
       <c r="W6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="X6" t="s">
         <v>89</v>
@@ -1395,8 +1412,11 @@
       <c r="Y6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1434,43 +1454,46 @@
         <v>57</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="s">
-        <v>58</v>
-      </c>
       <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" t="s">
         <v>3</v>
       </c>
-      <c r="R7" t="s">
-        <v>58</v>
-      </c>
       <c r="S7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U7" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="V7" t="s">
         <v>80</v>
       </c>
       <c r="W7" t="s">
+        <v>80</v>
+      </c>
+      <c r="X7" t="s">
         <v>90</v>
       </c>
-      <c r="X7" t="s">
-        <v>58</v>
-      </c>
       <c r="Y7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1511,34 +1534,34 @@
         <v>63</v>
       </c>
       <c r="N8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" t="s">
         <v>63</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" t="s">
-        <v>58</v>
-      </c>
       <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s">
         <v>4</v>
       </c>
-      <c r="R8" t="s">
-        <v>58</v>
-      </c>
       <c r="S8" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" t="s">
         <v>63</v>
       </c>
-      <c r="T8" t="s">
-        <v>58</v>
-      </c>
       <c r="U8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="V8" t="s">
         <v>63</v>
       </c>
       <c r="W8" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="X8" t="s">
         <v>91</v>
@@ -1546,8 +1569,11 @@
       <c r="Y8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1585,34 +1611,34 @@
         <v>57</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
-        <v>58</v>
-      </c>
       <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s">
         <v>5</v>
       </c>
-      <c r="R9" t="s">
-        <v>58</v>
-      </c>
       <c r="S9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U9" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="V9" t="s">
         <v>80</v>
       </c>
-      <c r="W9" s="10" t="s">
-        <v>146</v>
+      <c r="W9" t="s">
+        <v>80</v>
       </c>
       <c r="X9" s="10" t="s">
         <v>146</v>
@@ -1620,8 +1646,11 @@
       <c r="Y9" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z9" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1661,35 +1690,32 @@
       <c r="M10" t="s">
         <v>63</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>63</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>39</v>
       </c>
-      <c r="P10" t="s">
-        <v>58</v>
-      </c>
       <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" t="s">
         <v>6</v>
       </c>
-      <c r="R10" t="s">
-        <v>58</v>
-      </c>
       <c r="S10" t="s">
+        <v>58</v>
+      </c>
+      <c r="T10" t="s">
         <v>63</v>
       </c>
-      <c r="T10" t="s">
-        <v>58</v>
-      </c>
       <c r="U10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="V10" t="s">
         <v>63</v>
       </c>
       <c r="W10" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="X10" t="s">
         <v>92</v>
@@ -1697,8 +1723,11 @@
       <c r="Y10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1733,34 +1762,34 @@
         <v>57</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" t="s">
         <v>38</v>
       </c>
-      <c r="P11" t="s">
-        <v>58</v>
-      </c>
       <c r="Q11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" t="s">
         <v>7</v>
       </c>
-      <c r="R11" t="s">
-        <v>58</v>
-      </c>
       <c r="S11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T11" t="s">
-        <v>58</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U11" t="s">
+        <v>58</v>
       </c>
       <c r="V11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W11" t="s">
-        <v>93</v>
+      <c r="W11" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X11" t="s">
         <v>93</v>
@@ -1768,8 +1797,11 @@
       <c r="Y11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1803,27 +1835,24 @@
       <c r="M12" t="s">
         <v>58</v>
       </c>
-      <c r="N12" t="s">
-        <v>58</v>
-      </c>
       <c r="O12" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" t="s">
         <v>37</v>
       </c>
-      <c r="P12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" t="s">
         <v>8</v>
       </c>
-      <c r="R12" t="s">
-        <v>58</v>
-      </c>
       <c r="S12" t="s">
+        <v>58</v>
+      </c>
+      <c r="T12" t="s">
         <v>69</v>
       </c>
-      <c r="T12" t="s">
-        <v>58</v>
-      </c>
       <c r="U12" t="s">
         <v>58</v>
       </c>
@@ -1831,7 +1860,7 @@
         <v>58</v>
       </c>
       <c r="W12" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="X12" t="s">
         <v>94</v>
@@ -1839,8 +1868,11 @@
       <c r="Y12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1875,34 +1907,34 @@
         <v>57</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O13" t="s">
+        <v>58</v>
+      </c>
+      <c r="P13" t="s">
         <v>38</v>
       </c>
-      <c r="P13" t="s">
-        <v>58</v>
-      </c>
       <c r="Q13" t="s">
+        <v>58</v>
+      </c>
+      <c r="R13" t="s">
         <v>9</v>
       </c>
-      <c r="R13" t="s">
-        <v>58</v>
-      </c>
       <c r="S13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T13" t="s">
-        <v>58</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U13" t="s">
+        <v>58</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W13" t="s">
-        <v>95</v>
+      <c r="W13" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X13" t="s">
         <v>95</v>
@@ -1910,8 +1942,11 @@
       <c r="Y13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1948,35 +1983,32 @@
       <c r="M14" t="s">
         <v>65</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>65</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>41</v>
       </c>
-      <c r="P14" t="s">
-        <v>58</v>
-      </c>
       <c r="Q14" t="s">
+        <v>58</v>
+      </c>
+      <c r="R14" t="s">
         <v>10</v>
       </c>
-      <c r="R14" t="s">
-        <v>58</v>
-      </c>
       <c r="S14" t="s">
+        <v>58</v>
+      </c>
+      <c r="T14" t="s">
         <v>65</v>
       </c>
-      <c r="T14" t="s">
-        <v>58</v>
-      </c>
       <c r="U14" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="V14" t="s">
         <v>81</v>
       </c>
       <c r="W14" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="X14" t="s">
         <v>96</v>
@@ -1984,8 +2016,11 @@
       <c r="Y14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2023,23 +2058,23 @@
         <v>58</v>
       </c>
       <c r="O15" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" t="s">
         <v>37</v>
       </c>
-      <c r="P15" t="s">
-        <v>58</v>
-      </c>
       <c r="Q15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R15" t="s">
         <v>11</v>
       </c>
-      <c r="R15" t="s">
-        <v>58</v>
-      </c>
       <c r="S15" t="s">
+        <v>58</v>
+      </c>
+      <c r="T15" t="s">
         <v>69</v>
       </c>
-      <c r="T15" t="s">
-        <v>58</v>
-      </c>
       <c r="U15" t="s">
         <v>58</v>
       </c>
@@ -2047,7 +2082,7 @@
         <v>58</v>
       </c>
       <c r="W15" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="X15" t="s">
         <v>97</v>
@@ -2055,8 +2090,11 @@
       <c r="Y15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2091,34 +2129,34 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P16" t="s">
         <v>38</v>
       </c>
-      <c r="P16" t="s">
-        <v>58</v>
-      </c>
       <c r="Q16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" t="s">
         <v>12</v>
       </c>
-      <c r="R16" t="s">
-        <v>58</v>
-      </c>
       <c r="S16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T16" t="s">
-        <v>58</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U16" t="s">
+        <v>58</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W16" t="s">
-        <v>98</v>
+      <c r="W16" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X16" t="s">
         <v>98</v>
@@ -2126,8 +2164,11 @@
       <c r="Y16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2165,23 +2206,23 @@
         <v>58</v>
       </c>
       <c r="O17" t="s">
+        <v>58</v>
+      </c>
+      <c r="P17" t="s">
         <v>37</v>
       </c>
-      <c r="P17" t="s">
-        <v>58</v>
-      </c>
       <c r="Q17" t="s">
+        <v>58</v>
+      </c>
+      <c r="R17" t="s">
         <v>13</v>
       </c>
-      <c r="R17" t="s">
-        <v>58</v>
-      </c>
       <c r="S17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T17" t="s">
         <v>69</v>
       </c>
-      <c r="T17" t="s">
-        <v>58</v>
-      </c>
       <c r="U17" t="s">
         <v>58</v>
       </c>
@@ -2189,7 +2230,7 @@
         <v>58</v>
       </c>
       <c r="W17" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="X17" t="s">
         <v>99</v>
@@ -2197,8 +2238,11 @@
       <c r="Y17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2233,43 +2277,46 @@
         <v>57</v>
       </c>
       <c r="N18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" t="s">
         <v>38</v>
       </c>
-      <c r="P18" t="s">
-        <v>58</v>
-      </c>
       <c r="Q18" t="s">
+        <v>58</v>
+      </c>
+      <c r="R18" t="s">
         <v>14</v>
       </c>
-      <c r="R18" t="s">
-        <v>58</v>
-      </c>
       <c r="S18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T18" t="s">
-        <v>58</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U18" t="s">
+        <v>58</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W18" s="10" t="s">
+      <c r="W18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X18" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="X18" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="Y18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z18" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2310,23 +2357,23 @@
         <v>58</v>
       </c>
       <c r="O19" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" t="s">
         <v>37</v>
       </c>
-      <c r="P19" t="s">
-        <v>58</v>
-      </c>
       <c r="Q19" t="s">
+        <v>58</v>
+      </c>
+      <c r="R19" t="s">
         <v>15</v>
       </c>
-      <c r="R19" t="s">
-        <v>58</v>
-      </c>
       <c r="S19" t="s">
+        <v>58</v>
+      </c>
+      <c r="T19" t="s">
         <v>69</v>
       </c>
-      <c r="T19" t="s">
-        <v>58</v>
-      </c>
       <c r="U19" t="s">
         <v>58</v>
       </c>
@@ -2334,7 +2381,7 @@
         <v>58</v>
       </c>
       <c r="W19" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="X19" t="s">
         <v>100</v>
@@ -2342,8 +2389,11 @@
       <c r="Y19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2378,34 +2428,34 @@
         <v>57</v>
       </c>
       <c r="N20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20" t="s">
         <v>38</v>
       </c>
-      <c r="P20" t="s">
-        <v>58</v>
-      </c>
       <c r="Q20" t="s">
+        <v>58</v>
+      </c>
+      <c r="R20" t="s">
         <v>16</v>
       </c>
-      <c r="R20" t="s">
-        <v>58</v>
-      </c>
       <c r="S20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T20" t="s">
-        <v>58</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U20" t="s">
+        <v>58</v>
       </c>
       <c r="V20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W20" t="s">
-        <v>101</v>
+      <c r="W20" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X20" t="s">
         <v>101</v>
@@ -2413,8 +2463,11 @@
       <c r="Y20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2455,31 +2508,31 @@
         <v>58</v>
       </c>
       <c r="O21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P21" t="s">
         <v>38</v>
       </c>
-      <c r="P21" t="s">
-        <v>58</v>
-      </c>
       <c r="Q21" t="s">
+        <v>58</v>
+      </c>
+      <c r="R21" t="s">
         <v>17</v>
       </c>
-      <c r="R21" t="s">
-        <v>58</v>
-      </c>
       <c r="S21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T21" t="s">
-        <v>58</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U21" t="s">
+        <v>58</v>
       </c>
       <c r="V21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W21" t="s">
-        <v>102</v>
+      <c r="W21" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X21" t="s">
         <v>102</v>
@@ -2487,8 +2540,11 @@
       <c r="Y21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2526,31 +2582,31 @@
         <v>58</v>
       </c>
       <c r="O22" t="s">
+        <v>58</v>
+      </c>
+      <c r="P22" t="s">
         <v>37</v>
       </c>
-      <c r="P22" t="s">
-        <v>58</v>
-      </c>
       <c r="Q22" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" t="s">
         <v>18</v>
       </c>
-      <c r="R22" t="s">
-        <v>58</v>
-      </c>
       <c r="S22" t="s">
+        <v>58</v>
+      </c>
+      <c r="T22" t="s">
         <v>69</v>
       </c>
-      <c r="T22" t="s">
-        <v>58</v>
-      </c>
-      <c r="U22" s="5" t="s">
+      <c r="U22" t="s">
         <v>58</v>
       </c>
       <c r="V22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W22" t="s">
-        <v>103</v>
+      <c r="W22" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="X22" t="s">
         <v>103</v>
@@ -2558,8 +2614,11 @@
       <c r="Y22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2600,31 +2659,31 @@
         <v>58</v>
       </c>
       <c r="O23" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23" t="s">
         <v>37</v>
       </c>
-      <c r="P23" t="s">
-        <v>58</v>
-      </c>
       <c r="Q23" t="s">
+        <v>58</v>
+      </c>
+      <c r="R23" t="s">
         <v>19</v>
       </c>
-      <c r="R23" t="s">
-        <v>58</v>
-      </c>
       <c r="S23" t="s">
+        <v>58</v>
+      </c>
+      <c r="T23" t="s">
         <v>59</v>
       </c>
-      <c r="T23" t="s">
-        <v>58</v>
-      </c>
-      <c r="U23" s="5" t="s">
+      <c r="U23" t="s">
         <v>58</v>
       </c>
       <c r="V23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W23" t="s">
-        <v>59</v>
+      <c r="W23" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="X23" t="s">
         <v>59</v>
@@ -2632,8 +2691,11 @@
       <c r="Y23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2671,34 +2733,34 @@
         <v>57</v>
       </c>
       <c r="N24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O24" t="s">
+        <v>58</v>
+      </c>
+      <c r="P24" t="s">
         <v>38</v>
       </c>
-      <c r="P24" t="s">
-        <v>58</v>
-      </c>
       <c r="Q24" t="s">
+        <v>58</v>
+      </c>
+      <c r="R24" t="s">
         <v>20</v>
       </c>
-      <c r="R24" t="s">
-        <v>58</v>
-      </c>
       <c r="S24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T24" t="s">
-        <v>58</v>
-      </c>
-      <c r="U24" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U24" t="s">
+        <v>58</v>
       </c>
       <c r="V24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W24" t="s">
-        <v>104</v>
+      <c r="W24" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X24" t="s">
         <v>104</v>
@@ -2706,8 +2768,11 @@
       <c r="Y24" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2745,34 +2810,34 @@
         <v>57</v>
       </c>
       <c r="N25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O25" t="s">
+        <v>58</v>
+      </c>
+      <c r="P25" t="s">
         <v>38</v>
       </c>
-      <c r="P25" t="s">
-        <v>58</v>
-      </c>
       <c r="Q25" t="s">
+        <v>58</v>
+      </c>
+      <c r="R25" t="s">
         <v>21</v>
       </c>
-      <c r="R25" t="s">
-        <v>58</v>
-      </c>
       <c r="S25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T25" t="s">
-        <v>58</v>
-      </c>
-      <c r="U25" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U25" t="s">
+        <v>58</v>
       </c>
       <c r="V25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W25" t="s">
-        <v>105</v>
+      <c r="W25" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X25" t="s">
         <v>105</v>
@@ -2780,8 +2845,11 @@
       <c r="Y25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2825,31 +2893,31 @@
         <v>58</v>
       </c>
       <c r="O26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P26" t="s">
         <v>39</v>
       </c>
-      <c r="P26" t="s">
-        <v>58</v>
-      </c>
       <c r="Q26" t="s">
+        <v>58</v>
+      </c>
+      <c r="R26" t="s">
         <v>22</v>
       </c>
-      <c r="R26" t="s">
-        <v>58</v>
-      </c>
       <c r="S26" t="s">
+        <v>58</v>
+      </c>
+      <c r="T26" t="s">
         <v>63</v>
       </c>
-      <c r="T26" t="s">
-        <v>58</v>
-      </c>
       <c r="U26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="V26" t="s">
         <v>63</v>
       </c>
       <c r="W26" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="X26" t="s">
         <v>106</v>
@@ -2857,8 +2925,11 @@
       <c r="Y26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2896,34 +2967,34 @@
         <v>57</v>
       </c>
       <c r="N27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O27" t="s">
+        <v>58</v>
+      </c>
+      <c r="P27" t="s">
         <v>42</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>51</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>23</v>
       </c>
-      <c r="R27" t="s">
-        <v>58</v>
-      </c>
       <c r="S27" t="s">
+        <v>58</v>
+      </c>
+      <c r="T27" t="s">
         <v>70</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>51</v>
-      </c>
-      <c r="U27" t="s">
-        <v>82</v>
       </c>
       <c r="V27" t="s">
         <v>82</v>
       </c>
       <c r="W27" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="X27" t="s">
         <v>107</v>
@@ -2931,8 +3002,11 @@
       <c r="Y27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2970,34 +3044,34 @@
         <v>57</v>
       </c>
       <c r="N28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" t="s">
         <v>38</v>
       </c>
-      <c r="P28" t="s">
-        <v>58</v>
-      </c>
       <c r="Q28" t="s">
+        <v>58</v>
+      </c>
+      <c r="R28" t="s">
         <v>24</v>
       </c>
-      <c r="R28" t="s">
-        <v>58</v>
-      </c>
       <c r="S28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T28" t="s">
-        <v>58</v>
-      </c>
-      <c r="U28" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U28" t="s">
+        <v>58</v>
       </c>
       <c r="V28" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W28" t="s">
-        <v>108</v>
+      <c r="W28" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X28" t="s">
         <v>108</v>
@@ -3005,8 +3079,11 @@
       <c r="Y28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3047,34 +3124,34 @@
         <v>63</v>
       </c>
       <c r="N29" t="s">
+        <v>58</v>
+      </c>
+      <c r="O29" t="s">
         <v>63</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>39</v>
       </c>
-      <c r="P29" t="s">
-        <v>58</v>
-      </c>
       <c r="Q29" t="s">
+        <v>58</v>
+      </c>
+      <c r="R29" t="s">
         <v>25</v>
       </c>
-      <c r="R29" t="s">
-        <v>58</v>
-      </c>
       <c r="S29" t="s">
+        <v>58</v>
+      </c>
+      <c r="T29" t="s">
         <v>63</v>
       </c>
-      <c r="T29" t="s">
-        <v>58</v>
-      </c>
       <c r="U29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="V29" t="s">
         <v>63</v>
       </c>
       <c r="W29" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="X29" t="s">
         <v>109</v>
@@ -3082,8 +3159,11 @@
       <c r="Y29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3120,35 +3200,32 @@
       <c r="M30" t="s">
         <v>58</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>66</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>43</v>
       </c>
-      <c r="P30" t="s">
-        <v>58</v>
-      </c>
       <c r="Q30" t="s">
+        <v>58</v>
+      </c>
+      <c r="R30" t="s">
         <v>26</v>
       </c>
-      <c r="R30" t="s">
-        <v>58</v>
-      </c>
       <c r="S30" t="s">
+        <v>58</v>
+      </c>
+      <c r="T30" t="s">
         <v>66</v>
       </c>
-      <c r="T30" t="s">
-        <v>58</v>
-      </c>
       <c r="U30" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="V30" t="s">
         <v>83</v>
       </c>
       <c r="W30" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="X30" t="s">
         <v>110</v>
@@ -3156,8 +3233,11 @@
       <c r="Y30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3197,35 +3277,32 @@
       <c r="M31" t="s">
         <v>62</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>62</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>44</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>48</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>27</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>48</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>62</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>52</v>
-      </c>
-      <c r="U31" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="V31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="W31" t="s">
-        <v>111</v>
+      <c r="W31" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="X31" t="s">
         <v>111</v>
@@ -3233,8 +3310,11 @@
       <c r="Y31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3272,34 +3352,34 @@
         <v>57</v>
       </c>
       <c r="N32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O32" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" t="s">
         <v>42</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>51</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>28</v>
       </c>
-      <c r="R32" t="s">
-        <v>58</v>
-      </c>
       <c r="S32" t="s">
+        <v>58</v>
+      </c>
+      <c r="T32" t="s">
         <v>70</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>51</v>
-      </c>
-      <c r="U32" t="s">
-        <v>82</v>
       </c>
       <c r="V32" t="s">
         <v>82</v>
       </c>
       <c r="W32" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="X32" t="s">
         <v>112</v>
@@ -3307,8 +3387,11 @@
       <c r="Y32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3346,34 +3429,34 @@
         <v>57</v>
       </c>
       <c r="N33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O33" t="s">
+        <v>58</v>
+      </c>
+      <c r="P33" t="s">
         <v>38</v>
       </c>
-      <c r="P33" t="s">
-        <v>58</v>
-      </c>
       <c r="Q33" t="s">
+        <v>58</v>
+      </c>
+      <c r="R33" t="s">
         <v>29</v>
       </c>
-      <c r="R33" t="s">
-        <v>58</v>
-      </c>
       <c r="S33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T33" t="s">
-        <v>58</v>
-      </c>
-      <c r="U33" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U33" t="s">
+        <v>58</v>
       </c>
       <c r="V33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W33" t="s">
-        <v>113</v>
+      <c r="W33" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X33" t="s">
         <v>113</v>
@@ -3381,8 +3464,11 @@
       <c r="Y33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3420,34 +3506,34 @@
         <v>57</v>
       </c>
       <c r="N34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O34" t="s">
+        <v>58</v>
+      </c>
+      <c r="P34" t="s">
         <v>38</v>
       </c>
-      <c r="P34" t="s">
-        <v>58</v>
-      </c>
       <c r="Q34" t="s">
+        <v>58</v>
+      </c>
+      <c r="R34" t="s">
         <v>30</v>
       </c>
-      <c r="R34" t="s">
-        <v>58</v>
-      </c>
       <c r="S34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T34" t="s">
-        <v>58</v>
-      </c>
-      <c r="U34" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U34" t="s">
+        <v>58</v>
       </c>
       <c r="V34" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W34" t="s">
-        <v>114</v>
+      <c r="W34" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X34" t="s">
         <v>114</v>
@@ -3455,8 +3541,11 @@
       <c r="Y34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3494,34 +3583,34 @@
         <v>57</v>
       </c>
       <c r="N35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" t="s">
         <v>38</v>
       </c>
-      <c r="P35" t="s">
-        <v>58</v>
-      </c>
       <c r="Q35" t="s">
+        <v>58</v>
+      </c>
+      <c r="R35" t="s">
         <v>31</v>
       </c>
-      <c r="R35" t="s">
-        <v>58</v>
-      </c>
       <c r="S35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T35" t="s">
-        <v>58</v>
-      </c>
-      <c r="U35" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="U35" t="s">
+        <v>58</v>
       </c>
       <c r="V35" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="W35" t="s">
-        <v>115</v>
+      <c r="W35" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="X35" t="s">
         <v>115</v>
@@ -3529,8 +3618,11 @@
       <c r="Y35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3568,23 +3660,23 @@
         <v>58</v>
       </c>
       <c r="O36" t="s">
+        <v>58</v>
+      </c>
+      <c r="P36" t="s">
         <v>37</v>
       </c>
-      <c r="P36" t="s">
-        <v>58</v>
-      </c>
       <c r="Q36" t="s">
+        <v>58</v>
+      </c>
+      <c r="R36" t="s">
         <v>32</v>
       </c>
-      <c r="R36" t="s">
-        <v>58</v>
-      </c>
       <c r="S36" t="s">
+        <v>58</v>
+      </c>
+      <c r="T36" t="s">
         <v>69</v>
       </c>
-      <c r="T36" t="s">
-        <v>58</v>
-      </c>
       <c r="U36" t="s">
         <v>58</v>
       </c>
@@ -3592,7 +3684,7 @@
         <v>58</v>
       </c>
       <c r="W36" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="X36" t="s">
         <v>116</v>
@@ -3600,8 +3692,11 @@
       <c r="Y36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3639,23 +3734,23 @@
         <v>58</v>
       </c>
       <c r="O37" t="s">
+        <v>58</v>
+      </c>
+      <c r="P37" t="s">
         <v>37</v>
       </c>
-      <c r="P37" t="s">
-        <v>58</v>
-      </c>
       <c r="Q37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R37" t="s">
         <v>33</v>
       </c>
-      <c r="R37" t="s">
-        <v>58</v>
-      </c>
       <c r="S37" t="s">
+        <v>58</v>
+      </c>
+      <c r="T37" t="s">
         <v>69</v>
       </c>
-      <c r="T37" t="s">
-        <v>58</v>
-      </c>
       <c r="U37" t="s">
         <v>58</v>
       </c>
@@ -3663,7 +3758,7 @@
         <v>58</v>
       </c>
       <c r="W37" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="X37" t="s">
         <v>117</v>
@@ -3671,8 +3766,11 @@
       <c r="Y37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3713,34 +3811,34 @@
         <v>68</v>
       </c>
       <c r="N38" t="s">
+        <v>58</v>
+      </c>
+      <c r="O38" t="s">
         <v>68</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>40</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>50</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>34</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>49</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>68</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>49</v>
-      </c>
-      <c r="U38" t="s">
-        <v>85</v>
       </c>
       <c r="V38" t="s">
         <v>85</v>
       </c>
       <c r="W38" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="X38" t="s">
         <v>118</v>
@@ -3748,8 +3846,11 @@
       <c r="Y38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3787,34 +3888,34 @@
         <v>58</v>
       </c>
       <c r="N39" t="s">
+        <v>58</v>
+      </c>
+      <c r="O39" t="s">
         <v>66</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>43</v>
       </c>
-      <c r="P39" t="s">
-        <v>58</v>
-      </c>
       <c r="Q39" t="s">
+        <v>58</v>
+      </c>
+      <c r="R39" t="s">
         <v>35</v>
       </c>
-      <c r="R39" t="s">
-        <v>58</v>
-      </c>
       <c r="S39" t="s">
+        <v>58</v>
+      </c>
+      <c r="T39" t="s">
         <v>66</v>
       </c>
-      <c r="T39" t="s">
-        <v>58</v>
-      </c>
       <c r="U39" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="V39" t="s">
         <v>83</v>
       </c>
       <c r="W39" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="X39" t="s">
         <v>119</v>
@@ -3822,8 +3923,11 @@
       <c r="Y39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3861,34 +3965,34 @@
         <v>60</v>
       </c>
       <c r="N40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O40" t="s">
+        <v>58</v>
+      </c>
+      <c r="P40" t="s">
         <v>42</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>51</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>36</v>
       </c>
-      <c r="R40" t="s">
-        <v>58</v>
-      </c>
       <c r="S40" t="s">
+        <v>58</v>
+      </c>
+      <c r="T40" t="s">
         <v>70</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>51</v>
-      </c>
-      <c r="U40" t="s">
-        <v>82</v>
       </c>
       <c r="V40" t="s">
         <v>82</v>
       </c>
       <c r="W40" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="X40" t="s">
         <v>120</v>
@@ -3896,8 +4000,11 @@
       <c r="Y40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3916,27 +4023,24 @@
       <c r="M41" t="s">
         <v>58</v>
       </c>
-      <c r="N41" t="s">
-        <v>58</v>
-      </c>
       <c r="O41" t="s">
+        <v>58</v>
+      </c>
+      <c r="P41" t="s">
         <v>47</v>
       </c>
-      <c r="P41" t="s">
-        <v>58</v>
-      </c>
       <c r="Q41" t="s">
+        <v>58</v>
+      </c>
+      <c r="R41" t="s">
         <v>46</v>
       </c>
-      <c r="R41" t="s">
-        <v>58</v>
-      </c>
       <c r="S41" t="s">
+        <v>58</v>
+      </c>
+      <c r="T41" t="s">
         <v>69</v>
       </c>
-      <c r="T41" t="s">
-        <v>58</v>
-      </c>
       <c r="U41" t="s">
         <v>58</v>
       </c>
@@ -3952,8 +4056,11 @@
       <c r="Y41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3969,15 +4076,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="P1:U1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Converted test results excel to CSV file
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232B2352-7152-4DC5-9110-FAC324EF4E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -502,7 +501,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,7 +704,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,26 +737,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,23 +772,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -982,14 +947,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added Thorium 1.7.1 results with VoiceOver on Mac
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-test-results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACFF7BF-FE4C-9248-B6DB-0B7712504B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32420" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
   <definedNames>
     <definedName name="Title_8e133929154a42a88c65db5298a3d721" localSheetId="0">results!$A$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="153">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -481,12 +482,18 @@
   </si>
   <si>
     <t>Spoken by VoiceOver (Aldiko Next on iOS)</t>
+  </si>
+  <si>
+    <t>Voice Over / Thorium 1.7.1 on Mac</t>
+  </si>
+  <si>
+    <t>"horizontal Splitter"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -603,6 +610,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -689,7 +699,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -722,9 +732,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,6 +784,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -932,124 +976,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.453125" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="25.453125" customWidth="1"/>
-    <col min="21" max="21" width="24.6328125" customWidth="1"/>
-    <col min="22" max="22" width="30.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="25.5" customWidth="1"/>
+    <col min="22" max="22" width="24.6640625" customWidth="1"/>
+    <col min="23" max="23" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="17" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="14" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="15"/>
+      <c r="U1" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-    </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="13"/>
       <c r="K2" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="19" t="s">
+      <c r="M2" s="17"/>
+      <c r="N2" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="21"/>
+      <c r="S2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="W2" s="12" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -1090,34 +1139,37 @@
         <v>133</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1152,17 +1204,17 @@
         <v>57</v>
       </c>
       <c r="N4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" t="s">
         <v>0</v>
       </c>
-      <c r="O4" t="s">
-        <v>57</v>
-      </c>
       <c r="P4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" t="s">
-        <v>57</v>
-      </c>
       <c r="R4" t="s">
         <v>57</v>
       </c>
@@ -1170,7 +1222,7 @@
         <v>57</v>
       </c>
       <c r="T4" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="U4" t="s">
         <v>85</v>
@@ -1178,8 +1230,11 @@
       <c r="V4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1217,25 +1272,25 @@
         <v>57</v>
       </c>
       <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
-        <v>57</v>
-      </c>
       <c r="P5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="S5" t="s">
         <v>78</v>
       </c>
       <c r="T5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="U5" t="s">
         <v>86</v>
@@ -1243,8 +1298,11 @@
       <c r="V5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1283,25 +1341,25 @@
         <v>57</v>
       </c>
       <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" t="s">
         <v>2</v>
       </c>
-      <c r="O6" t="s">
-        <v>57</v>
-      </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R6" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="S6" t="s">
         <v>78</v>
       </c>
       <c r="T6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="U6" t="s">
         <v>87</v>
@@ -1309,8 +1367,11 @@
       <c r="V6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1348,34 +1409,37 @@
         <v>57</v>
       </c>
       <c r="N7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" t="s">
         <v>3</v>
       </c>
-      <c r="O7" t="s">
-        <v>57</v>
-      </c>
       <c r="P7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R7" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="S7" t="s">
         <v>78</v>
       </c>
       <c r="T7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U7" t="s">
         <v>88</v>
       </c>
-      <c r="U7" t="s">
-        <v>57</v>
-      </c>
       <c r="V7" t="s">
+        <v>57</v>
+      </c>
+      <c r="W7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1416,25 +1480,25 @@
         <v>57</v>
       </c>
       <c r="N8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" t="s">
         <v>4</v>
       </c>
-      <c r="O8" t="s">
-        <v>57</v>
-      </c>
       <c r="P8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q8" t="s">
         <v>61</v>
       </c>
-      <c r="Q8" t="s">
-        <v>57</v>
-      </c>
       <c r="R8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="S8" t="s">
         <v>61</v>
       </c>
       <c r="T8" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="U8" t="s">
         <v>89</v>
@@ -1442,8 +1506,11 @@
       <c r="V8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1481,25 +1548,25 @@
         <v>57</v>
       </c>
       <c r="N9" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" t="s">
         <v>5</v>
       </c>
-      <c r="O9" t="s">
-        <v>57</v>
-      </c>
       <c r="P9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R9" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="S9" t="s">
         <v>78</v>
       </c>
-      <c r="T9" s="10" t="s">
-        <v>140</v>
+      <c r="T9" t="s">
+        <v>78</v>
       </c>
       <c r="U9" s="10" t="s">
         <v>140</v>
@@ -1507,8 +1574,11 @@
       <c r="V9" s="10" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W9" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1546,25 +1616,25 @@
         <v>57</v>
       </c>
       <c r="N10" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" t="s">
         <v>6</v>
       </c>
-      <c r="O10" t="s">
-        <v>57</v>
-      </c>
       <c r="P10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s">
         <v>61</v>
       </c>
-      <c r="Q10" t="s">
-        <v>57</v>
-      </c>
       <c r="R10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="S10" t="s">
         <v>61</v>
       </c>
       <c r="T10" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="U10" t="s">
         <v>90</v>
@@ -1572,8 +1642,11 @@
       <c r="V10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1607,26 +1680,26 @@
       <c r="M11" t="s">
         <v>57</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" t="s">
         <v>7</v>
       </c>
-      <c r="O11" t="s">
-        <v>57</v>
-      </c>
       <c r="P11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q11" t="s">
-        <v>57</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R11" t="s">
+        <v>57</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T11" t="s">
-        <v>91</v>
+      <c r="T11" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U11" t="s">
         <v>91</v>
@@ -1634,8 +1707,11 @@
       <c r="V11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1666,18 +1742,18 @@
       <c r="M12" t="s">
         <v>57</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" t="s">
         <v>8</v>
       </c>
-      <c r="O12" t="s">
-        <v>57</v>
-      </c>
       <c r="P12" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q12" t="s">
         <v>67</v>
       </c>
-      <c r="Q12" t="s">
-        <v>57</v>
-      </c>
       <c r="R12" t="s">
         <v>57</v>
       </c>
@@ -1685,7 +1761,7 @@
         <v>57</v>
       </c>
       <c r="T12" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="U12" t="s">
         <v>92</v>
@@ -1693,8 +1769,11 @@
       <c r="V12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1728,26 +1807,26 @@
       <c r="M13" t="s">
         <v>57</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" t="s">
         <v>9</v>
       </c>
-      <c r="O13" t="s">
-        <v>57</v>
-      </c>
       <c r="P13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q13" t="s">
-        <v>57</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R13" t="s">
+        <v>57</v>
       </c>
       <c r="S13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T13" t="s">
-        <v>93</v>
+      <c r="T13" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U13" t="s">
         <v>93</v>
@@ -1755,8 +1834,11 @@
       <c r="V13" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1791,25 +1873,25 @@
         <v>57</v>
       </c>
       <c r="N14" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" t="s">
         <v>10</v>
       </c>
-      <c r="O14" t="s">
-        <v>57</v>
-      </c>
       <c r="P14" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14" t="s">
         <v>63</v>
       </c>
-      <c r="Q14" t="s">
-        <v>57</v>
-      </c>
       <c r="R14" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="S14" t="s">
         <v>79</v>
       </c>
       <c r="T14" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="U14" t="s">
         <v>94</v>
@@ -1817,8 +1899,11 @@
       <c r="V14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1852,18 +1937,18 @@
       <c r="M15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" t="s">
         <v>11</v>
       </c>
-      <c r="O15" t="s">
-        <v>57</v>
-      </c>
       <c r="P15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q15" t="s">
         <v>67</v>
       </c>
-      <c r="Q15" t="s">
-        <v>57</v>
-      </c>
       <c r="R15" t="s">
         <v>57</v>
       </c>
@@ -1871,7 +1956,7 @@
         <v>57</v>
       </c>
       <c r="T15" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="U15" t="s">
         <v>95</v>
@@ -1879,8 +1964,11 @@
       <c r="V15" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1914,26 +2002,26 @@
       <c r="M16" t="s">
         <v>57</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" t="s">
         <v>12</v>
       </c>
-      <c r="O16" t="s">
-        <v>57</v>
-      </c>
       <c r="P16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q16" t="s">
-        <v>57</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R16" t="s">
+        <v>57</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T16" t="s">
-        <v>96</v>
+      <c r="T16" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U16" t="s">
         <v>96</v>
@@ -1941,8 +2029,11 @@
       <c r="V16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1976,18 +2067,18 @@
       <c r="M17" t="s">
         <v>57</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" t="s">
         <v>13</v>
       </c>
-      <c r="O17" t="s">
-        <v>57</v>
-      </c>
       <c r="P17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" t="s">
         <v>67</v>
       </c>
-      <c r="Q17" t="s">
-        <v>57</v>
-      </c>
       <c r="R17" t="s">
         <v>57</v>
       </c>
@@ -1995,7 +2086,7 @@
         <v>57</v>
       </c>
       <c r="T17" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="U17" t="s">
         <v>97</v>
@@ -2003,8 +2094,11 @@
       <c r="V17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2038,35 +2132,38 @@
       <c r="M18" t="s">
         <v>57</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O18" t="s">
         <v>14</v>
       </c>
-      <c r="O18" t="s">
-        <v>57</v>
-      </c>
       <c r="P18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q18" t="s">
-        <v>57</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R18" t="s">
+        <v>57</v>
       </c>
       <c r="S18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="U18" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="U18" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="V18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W18" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2103,18 +2200,18 @@
       <c r="M19" t="s">
         <v>57</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O19" t="s">
         <v>15</v>
       </c>
-      <c r="O19" t="s">
-        <v>57</v>
-      </c>
       <c r="P19" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q19" t="s">
         <v>67</v>
       </c>
-      <c r="Q19" t="s">
-        <v>57</v>
-      </c>
       <c r="R19" t="s">
         <v>57</v>
       </c>
@@ -2122,7 +2219,7 @@
         <v>57</v>
       </c>
       <c r="T19" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="U19" t="s">
         <v>98</v>
@@ -2130,8 +2227,11 @@
       <c r="V19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2165,26 +2265,26 @@
       <c r="M20" t="s">
         <v>57</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O20" t="s">
         <v>16</v>
       </c>
-      <c r="O20" t="s">
-        <v>57</v>
-      </c>
       <c r="P20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R20" t="s">
+        <v>57</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T20" t="s">
-        <v>99</v>
+      <c r="T20" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U20" t="s">
         <v>99</v>
@@ -2192,8 +2292,11 @@
       <c r="V20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2230,26 +2333,26 @@
       <c r="M21" t="s">
         <v>57</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O21" t="s">
         <v>17</v>
       </c>
-      <c r="O21" t="s">
-        <v>57</v>
-      </c>
       <c r="P21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q21" t="s">
-        <v>57</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R21" t="s">
+        <v>57</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T21" t="s">
-        <v>100</v>
+      <c r="T21" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U21" t="s">
         <v>100</v>
@@ -2257,8 +2360,11 @@
       <c r="V21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2292,26 +2398,26 @@
       <c r="M22" t="s">
         <v>57</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O22" t="s">
         <v>18</v>
       </c>
-      <c r="O22" t="s">
-        <v>57</v>
-      </c>
       <c r="P22" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q22" t="s">
         <v>67</v>
       </c>
-      <c r="Q22" t="s">
-        <v>57</v>
-      </c>
-      <c r="R22" s="5" t="s">
+      <c r="R22" t="s">
         <v>57</v>
       </c>
       <c r="S22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="T22" t="s">
-        <v>101</v>
+      <c r="T22" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="U22" t="s">
         <v>101</v>
@@ -2319,8 +2425,11 @@
       <c r="V22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2357,26 +2466,26 @@
       <c r="M23" t="s">
         <v>57</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" t="s">
         <v>19</v>
       </c>
-      <c r="O23" t="s">
-        <v>57</v>
-      </c>
       <c r="P23" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q23" t="s">
         <v>58</v>
       </c>
-      <c r="Q23" t="s">
-        <v>57</v>
-      </c>
-      <c r="R23" s="5" t="s">
+      <c r="R23" t="s">
         <v>57</v>
       </c>
       <c r="S23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="T23" t="s">
-        <v>58</v>
+      <c r="T23" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="U23" t="s">
         <v>58</v>
@@ -2384,8 +2493,11 @@
       <c r="V23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2422,26 +2534,26 @@
       <c r="M24" t="s">
         <v>57</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" t="s">
         <v>20</v>
       </c>
-      <c r="O24" t="s">
-        <v>57</v>
-      </c>
       <c r="P24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q24" t="s">
-        <v>57</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R24" t="s">
+        <v>57</v>
       </c>
       <c r="S24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T24" t="s">
-        <v>102</v>
+      <c r="T24" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U24" t="s">
         <v>102</v>
@@ -2449,8 +2561,11 @@
       <c r="V24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2487,26 +2602,26 @@
       <c r="M25" t="s">
         <v>57</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="O25" t="s">
-        <v>57</v>
-      </c>
       <c r="P25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q25" t="s">
-        <v>57</v>
-      </c>
-      <c r="R25" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R25" t="s">
+        <v>57</v>
       </c>
       <c r="S25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T25" t="s">
-        <v>103</v>
+      <c r="T25" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U25" t="s">
         <v>103</v>
@@ -2514,8 +2629,11 @@
       <c r="V25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2556,25 +2674,25 @@
         <v>57</v>
       </c>
       <c r="N26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O26" t="s">
         <v>22</v>
       </c>
-      <c r="O26" t="s">
-        <v>57</v>
-      </c>
       <c r="P26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q26" t="s">
         <v>61</v>
       </c>
-      <c r="Q26" t="s">
-        <v>57</v>
-      </c>
       <c r="R26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="S26" t="s">
         <v>61</v>
       </c>
       <c r="T26" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="U26" t="s">
         <v>104</v>
@@ -2582,8 +2700,11 @@
       <c r="V26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2620,26 +2741,26 @@
       <c r="M27" t="s">
         <v>51</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O27" t="s">
         <v>23</v>
       </c>
-      <c r="O27" t="s">
-        <v>57</v>
-      </c>
       <c r="P27" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q27" t="s">
         <v>68</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>51</v>
-      </c>
-      <c r="R27" t="s">
-        <v>80</v>
       </c>
       <c r="S27" t="s">
         <v>80</v>
       </c>
       <c r="T27" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="U27" t="s">
         <v>105</v>
@@ -2647,8 +2768,11 @@
       <c r="V27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2685,26 +2809,26 @@
       <c r="M28" t="s">
         <v>57</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O28" t="s">
         <v>24</v>
       </c>
-      <c r="O28" t="s">
-        <v>57</v>
-      </c>
       <c r="P28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q28" t="s">
-        <v>57</v>
-      </c>
-      <c r="R28" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R28" t="s">
+        <v>57</v>
       </c>
       <c r="S28" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T28" t="s">
-        <v>106</v>
+      <c r="T28" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U28" t="s">
         <v>106</v>
@@ -2712,8 +2836,11 @@
       <c r="V28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2753,26 +2880,26 @@
       <c r="M29" t="s">
         <v>57</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O29" t="s">
         <v>25</v>
       </c>
-      <c r="O29" t="s">
-        <v>57</v>
-      </c>
       <c r="P29" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q29" t="s">
         <v>61</v>
       </c>
-      <c r="Q29" t="s">
-        <v>57</v>
-      </c>
       <c r="R29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="S29" t="s">
         <v>61</v>
       </c>
       <c r="T29" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="U29" t="s">
         <v>107</v>
@@ -2780,8 +2907,11 @@
       <c r="V29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2815,26 +2945,26 @@
       <c r="M30" t="s">
         <v>57</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O30" t="s">
         <v>26</v>
       </c>
-      <c r="O30" t="s">
-        <v>57</v>
-      </c>
       <c r="P30" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q30" t="s">
         <v>64</v>
       </c>
-      <c r="Q30" t="s">
-        <v>57</v>
-      </c>
       <c r="R30" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="S30" t="s">
         <v>81</v>
       </c>
       <c r="T30" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="U30" t="s">
         <v>108</v>
@@ -2842,8 +2972,11 @@
       <c r="V30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2880,26 +3013,26 @@
       <c r="M31" t="s">
         <v>48</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="O31" t="s">
         <v>27</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>48</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>60</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>52</v>
-      </c>
-      <c r="R31" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="S31" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="T31" t="s">
-        <v>109</v>
+      <c r="T31" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="U31" t="s">
         <v>109</v>
@@ -2907,8 +3040,11 @@
       <c r="V31" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2945,26 +3081,26 @@
       <c r="M32" t="s">
         <v>51</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" t="s">
         <v>28</v>
       </c>
-      <c r="O32" t="s">
-        <v>57</v>
-      </c>
       <c r="P32" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q32" t="s">
         <v>68</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>51</v>
-      </c>
-      <c r="R32" t="s">
-        <v>80</v>
       </c>
       <c r="S32" t="s">
         <v>80</v>
       </c>
       <c r="T32" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="U32" t="s">
         <v>110</v>
@@ -2972,8 +3108,11 @@
       <c r="V32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3010,26 +3149,26 @@
       <c r="M33" t="s">
         <v>57</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O33" t="s">
         <v>29</v>
       </c>
-      <c r="O33" t="s">
-        <v>57</v>
-      </c>
       <c r="P33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q33" t="s">
-        <v>57</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R33" t="s">
+        <v>57</v>
       </c>
       <c r="S33" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T33" t="s">
-        <v>111</v>
+      <c r="T33" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U33" t="s">
         <v>111</v>
@@ -3037,8 +3176,11 @@
       <c r="V33" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3075,26 +3217,26 @@
       <c r="M34" t="s">
         <v>57</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O34" t="s">
         <v>30</v>
       </c>
-      <c r="O34" t="s">
-        <v>57</v>
-      </c>
       <c r="P34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q34" t="s">
-        <v>57</v>
-      </c>
-      <c r="R34" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R34" t="s">
+        <v>57</v>
       </c>
       <c r="S34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T34" t="s">
-        <v>112</v>
+      <c r="T34" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U34" t="s">
         <v>112</v>
@@ -3102,8 +3244,11 @@
       <c r="V34" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3140,26 +3285,26 @@
       <c r="M35" t="s">
         <v>57</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O35" t="s">
         <v>31</v>
       </c>
-      <c r="O35" t="s">
-        <v>57</v>
-      </c>
       <c r="P35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q35" t="s">
-        <v>57</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="R35" t="s">
+        <v>57</v>
       </c>
       <c r="S35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T35" t="s">
-        <v>113</v>
+      <c r="T35" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="U35" t="s">
         <v>113</v>
@@ -3167,8 +3312,11 @@
       <c r="V35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3202,18 +3350,18 @@
       <c r="M36" t="s">
         <v>57</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O36" t="s">
         <v>32</v>
       </c>
-      <c r="O36" t="s">
-        <v>57</v>
-      </c>
       <c r="P36" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q36" t="s">
         <v>67</v>
       </c>
-      <c r="Q36" t="s">
-        <v>57</v>
-      </c>
       <c r="R36" t="s">
         <v>57</v>
       </c>
@@ -3221,7 +3369,7 @@
         <v>57</v>
       </c>
       <c r="T36" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="U36" t="s">
         <v>114</v>
@@ -3229,8 +3377,11 @@
       <c r="V36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3264,18 +3415,18 @@
       <c r="M37" t="s">
         <v>57</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O37" t="s">
         <v>33</v>
       </c>
-      <c r="O37" t="s">
-        <v>57</v>
-      </c>
       <c r="P37" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q37" t="s">
         <v>67</v>
       </c>
-      <c r="Q37" t="s">
-        <v>57</v>
-      </c>
       <c r="R37" t="s">
         <v>57</v>
       </c>
@@ -3283,7 +3434,7 @@
         <v>57</v>
       </c>
       <c r="T37" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="U37" t="s">
         <v>115</v>
@@ -3291,8 +3442,11 @@
       <c r="V37" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3333,25 +3487,25 @@
         <v>50</v>
       </c>
       <c r="N38" t="s">
+        <v>66</v>
+      </c>
+      <c r="O38" t="s">
         <v>34</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>49</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>66</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>49</v>
-      </c>
-      <c r="R38" t="s">
-        <v>83</v>
       </c>
       <c r="S38" t="s">
         <v>83</v>
       </c>
       <c r="T38" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="U38" t="s">
         <v>116</v>
@@ -3359,8 +3513,11 @@
       <c r="V38" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3397,26 +3554,26 @@
       <c r="M39" t="s">
         <v>57</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O39" t="s">
         <v>35</v>
       </c>
-      <c r="O39" t="s">
-        <v>57</v>
-      </c>
       <c r="P39" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q39" t="s">
         <v>64</v>
       </c>
-      <c r="Q39" t="s">
-        <v>57</v>
-      </c>
       <c r="R39" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="S39" t="s">
         <v>81</v>
       </c>
       <c r="T39" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="U39" t="s">
         <v>117</v>
@@ -3424,8 +3581,11 @@
       <c r="V39" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3462,26 +3622,26 @@
       <c r="M40" t="s">
         <v>51</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" t="s">
         <v>36</v>
       </c>
-      <c r="O40" t="s">
-        <v>57</v>
-      </c>
       <c r="P40" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q40" t="s">
         <v>68</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>51</v>
-      </c>
-      <c r="R40" t="s">
-        <v>80</v>
       </c>
       <c r="S40" t="s">
         <v>80</v>
       </c>
       <c r="T40" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="U40" t="s">
         <v>118</v>
@@ -3489,8 +3649,11 @@
       <c r="V40" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3512,18 +3675,18 @@
       <c r="M41" t="s">
         <v>57</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O41" t="s">
         <v>46</v>
       </c>
-      <c r="O41" t="s">
-        <v>57</v>
-      </c>
       <c r="P41" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q41" t="s">
         <v>67</v>
       </c>
-      <c r="Q41" t="s">
-        <v>57</v>
-      </c>
       <c r="R41" t="s">
         <v>57</v>
       </c>
@@ -3539,8 +3702,11 @@
       <c r="V41" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3553,15 +3719,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="B1:K1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="L1:R1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>